<commit_message>
Added heatmap information for grouping Industries
</commit_message>
<xml_diff>
--- a/mexico.xlsx
+++ b/mexico.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="395">
   <si>
     <t>date</t>
   </si>
@@ -1193,6 +1193,9 @@
   </si>
   <si>
     <t>2021-02-13</t>
+  </si>
+  <si>
+    <t>2021-02-14</t>
   </si>
   <si>
     <t>mexico</t>
@@ -1553,7 +1556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E390"/>
+  <dimension ref="A1:E391"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1581,7 +1584,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1598,7 +1601,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1615,7 +1618,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1632,7 +1635,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1649,7 +1652,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1666,7 +1669,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1683,7 +1686,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1700,7 +1703,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1717,7 +1720,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1734,7 +1737,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1751,7 +1754,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1768,7 +1771,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1785,7 +1788,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1802,7 +1805,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1819,7 +1822,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1836,7 +1839,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1853,7 +1856,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1870,7 +1873,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1887,7 +1890,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1904,7 +1907,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1921,7 +1924,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1938,7 +1941,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1955,7 +1958,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1972,7 +1975,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1989,7 +1992,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2006,7 +2009,7 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2023,7 +2026,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2040,7 +2043,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2057,7 +2060,7 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2074,7 +2077,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2091,7 +2094,7 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2108,7 +2111,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2125,7 +2128,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2142,7 +2145,7 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2159,7 +2162,7 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2176,7 +2179,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2193,7 +2196,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2210,7 +2213,7 @@
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2227,7 +2230,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -2244,7 +2247,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D41">
         <v>5</v>
@@ -2261,7 +2264,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D42">
         <v>5</v>
@@ -2278,7 +2281,7 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2295,7 +2298,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D44">
         <v>5</v>
@@ -2312,7 +2315,7 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D45">
         <v>5</v>
@@ -2329,7 +2332,7 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D46">
         <v>6</v>
@@ -2346,7 +2349,7 @@
         <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D47">
         <v>6</v>
@@ -2363,7 +2366,7 @@
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D48">
         <v>7</v>
@@ -2380,7 +2383,7 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D49">
         <v>7</v>
@@ -2397,7 +2400,7 @@
         <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D50">
         <v>7</v>
@@ -2414,7 +2417,7 @@
         <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D51">
         <v>8</v>
@@ -2431,7 +2434,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D52">
         <v>12</v>
@@ -2448,7 +2451,7 @@
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D53">
         <v>26</v>
@@ -2465,7 +2468,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D54">
         <v>41</v>
@@ -2482,7 +2485,7 @@
         <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D55">
         <v>53</v>
@@ -2499,7 +2502,7 @@
         <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D56">
         <v>82</v>
@@ -2516,7 +2519,7 @@
         <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D57">
         <v>93</v>
@@ -2533,7 +2536,7 @@
         <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D58">
         <v>118</v>
@@ -2550,7 +2553,7 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D59">
         <v>164</v>
@@ -2567,7 +2570,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D60">
         <v>203</v>
@@ -2584,7 +2587,7 @@
         <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D61">
         <v>251</v>
@@ -2601,7 +2604,7 @@
         <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D62">
         <v>316</v>
@@ -2618,7 +2621,7 @@
         <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D63">
         <v>367</v>
@@ -2635,7 +2638,7 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D64">
         <v>405</v>
@@ -2652,7 +2655,7 @@
         <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D65">
         <v>475</v>
@@ -2669,7 +2672,7 @@
         <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D66">
         <v>585</v>
@@ -2686,7 +2689,7 @@
         <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D67">
         <v>717</v>
@@ -2703,7 +2706,7 @@
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D68">
         <v>848</v>
@@ -2720,7 +2723,7 @@
         <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D69">
         <v>993</v>
@@ -2737,7 +2740,7 @@
         <v>72</v>
       </c>
       <c r="C70" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D70">
         <v>1094</v>
@@ -2754,7 +2757,7 @@
         <v>73</v>
       </c>
       <c r="C71" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D71">
         <v>1215</v>
@@ -2771,7 +2774,7 @@
         <v>74</v>
       </c>
       <c r="C72" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D72">
         <v>1378</v>
@@ -2788,7 +2791,7 @@
         <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D73">
         <v>1510</v>
@@ -2805,7 +2808,7 @@
         <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D74">
         <v>1688</v>
@@ -2822,7 +2825,7 @@
         <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D75">
         <v>1890</v>
@@ -2839,7 +2842,7 @@
         <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D76">
         <v>2143</v>
@@ -2856,7 +2859,7 @@
         <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D77">
         <v>2439</v>
@@ -2873,7 +2876,7 @@
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D78">
         <v>2785</v>
@@ -2890,7 +2893,7 @@
         <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D79">
         <v>3181</v>
@@ -2907,7 +2910,7 @@
         <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D80">
         <v>3441</v>
@@ -2924,7 +2927,7 @@
         <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D81">
         <v>3844</v>
@@ -2941,7 +2944,7 @@
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D82">
         <v>4219</v>
@@ -2958,7 +2961,7 @@
         <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D83">
         <v>4661</v>
@@ -2975,7 +2978,7 @@
         <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D84">
         <v>5014</v>
@@ -2992,7 +2995,7 @@
         <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D85">
         <v>5399</v>
@@ -3009,7 +3012,7 @@
         <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D86">
         <v>5847</v>
@@ -3026,7 +3029,7 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D87">
         <v>6297</v>
@@ -3043,7 +3046,7 @@
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D88">
         <v>6875</v>
@@ -3060,7 +3063,7 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D89">
         <v>7497</v>
@@ -3077,7 +3080,7 @@
         <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D90">
         <v>8261</v>
@@ -3094,7 +3097,7 @@
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D91">
         <v>8772</v>
@@ -3111,7 +3114,7 @@
         <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D92">
         <v>9501</v>
@@ -3128,7 +3131,7 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D93">
         <v>10544</v>
@@ -3145,7 +3148,7 @@
         <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D94">
         <v>11633</v>
@@ -3162,7 +3165,7 @@
         <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D95">
         <v>12872</v>
@@ -3179,7 +3182,7 @@
         <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D96">
         <v>13842</v>
@@ -3196,7 +3199,7 @@
         <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D97">
         <v>14677</v>
@@ -3213,7 +3216,7 @@
         <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D98">
         <v>15529</v>
@@ -3230,7 +3233,7 @@
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D99">
         <v>16752</v>
@@ -3247,7 +3250,7 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D100">
         <v>17799</v>
@@ -3264,7 +3267,7 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D101">
         <v>19224</v>
@@ -3281,7 +3284,7 @@
         <v>104</v>
       </c>
       <c r="C102" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D102">
         <v>20739</v>
@@ -3298,7 +3301,7 @@
         <v>105</v>
       </c>
       <c r="C103" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D103">
         <v>22088</v>
@@ -3315,7 +3318,7 @@
         <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D104">
         <v>23471</v>
@@ -3332,7 +3335,7 @@
         <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D105">
         <v>24905</v>
@@ -3349,7 +3352,7 @@
         <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D106">
         <v>26025</v>
@@ -3366,7 +3369,7 @@
         <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D107">
         <v>27634</v>
@@ -3383,7 +3386,7 @@
         <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D108">
         <v>29616</v>
@@ -3400,7 +3403,7 @@
         <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D109">
         <v>31522</v>
@@ -3417,7 +3420,7 @@
         <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D110">
         <v>33460</v>
@@ -3434,7 +3437,7 @@
         <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D111">
         <v>35022</v>
@@ -3451,7 +3454,7 @@
         <v>114</v>
       </c>
       <c r="C112" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D112">
         <v>36327</v>
@@ -3468,7 +3471,7 @@
         <v>115</v>
       </c>
       <c r="C113" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D113">
         <v>38324</v>
@@ -3485,7 +3488,7 @@
         <v>116</v>
       </c>
       <c r="C114" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D114">
         <v>40186</v>
@@ -3502,7 +3505,7 @@
         <v>117</v>
       </c>
       <c r="C115" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D115">
         <v>42595</v>
@@ -3519,7 +3522,7 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D116">
         <v>45032</v>
@@ -3536,7 +3539,7 @@
         <v>119</v>
       </c>
       <c r="C117" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D117">
         <v>47144</v>
@@ -3553,7 +3556,7 @@
         <v>120</v>
       </c>
       <c r="C118" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D118">
         <v>49219</v>
@@ -3570,7 +3573,7 @@
         <v>121</v>
       </c>
       <c r="C119" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D119">
         <v>51633</v>
@@ -3587,7 +3590,7 @@
         <v>122</v>
       </c>
       <c r="C120" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D120">
         <v>54346</v>
@@ -3604,7 +3607,7 @@
         <v>123</v>
       </c>
       <c r="C121" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D121">
         <v>56594</v>
@@ -3621,7 +3624,7 @@
         <v>124</v>
       </c>
       <c r="C122" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D122">
         <v>59567</v>
@@ -3638,7 +3641,7 @@
         <v>125</v>
       </c>
       <c r="C123" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D123">
         <v>62527</v>
@@ -3655,7 +3658,7 @@
         <v>126</v>
       </c>
       <c r="C124" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D124">
         <v>65856</v>
@@ -3672,7 +3675,7 @@
         <v>127</v>
       </c>
       <c r="C125" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D125">
         <v>68620</v>
@@ -3689,7 +3692,7 @@
         <v>128</v>
       </c>
       <c r="C126" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D126">
         <v>71105</v>
@@ -3706,7 +3709,7 @@
         <v>129</v>
       </c>
       <c r="C127" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D127">
         <v>74560</v>
@@ -3723,7 +3726,7 @@
         <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D128">
         <v>78023</v>
@@ -3740,7 +3743,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D129">
         <v>81400</v>
@@ -3757,7 +3760,7 @@
         <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D130">
         <v>84627</v>
@@ -3774,7 +3777,7 @@
         <v>133</v>
       </c>
       <c r="C131" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D131">
         <v>87512</v>
@@ -3791,7 +3794,7 @@
         <v>134</v>
       </c>
       <c r="C132" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D132">
         <v>90664</v>
@@ -3808,7 +3811,7 @@
         <v>135</v>
       </c>
       <c r="C133" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D133">
         <v>93435</v>
@@ -3825,7 +3828,7 @@
         <v>136</v>
       </c>
       <c r="C134" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D134">
         <v>97326</v>
@@ -3842,7 +3845,7 @@
         <v>137</v>
       </c>
       <c r="C135" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D135">
         <v>101238</v>
@@ -3859,7 +3862,7 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D136">
         <v>105680</v>
@@ -3876,7 +3879,7 @@
         <v>139</v>
       </c>
       <c r="C137" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D137">
         <v>110026</v>
@@ -3893,7 +3896,7 @@
         <v>140</v>
       </c>
       <c r="C138" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D138">
         <v>113619</v>
@@ -3910,7 +3913,7 @@
         <v>141</v>
       </c>
       <c r="C139" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D139">
         <v>117103</v>
@@ -3927,7 +3930,7 @@
         <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D140">
         <v>120102</v>
@@ -3944,7 +3947,7 @@
         <v>143</v>
       </c>
       <c r="C141" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D141">
         <v>124301</v>
@@ -3961,7 +3964,7 @@
         <v>144</v>
       </c>
       <c r="C142" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D142">
         <v>129184</v>
@@ -3978,7 +3981,7 @@
         <v>145</v>
       </c>
       <c r="C143" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D143">
         <v>133974</v>
@@ -3995,7 +3998,7 @@
         <v>146</v>
       </c>
       <c r="C144" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D144">
         <v>139196</v>
@@ -4012,7 +4015,7 @@
         <v>147</v>
       </c>
       <c r="C145" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D145">
         <v>142690</v>
@@ -4029,7 +4032,7 @@
         <v>148</v>
       </c>
       <c r="C146" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D146">
         <v>146837</v>
@@ -4046,7 +4049,7 @@
         <v>149</v>
       </c>
       <c r="C147" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D147">
         <v>150264</v>
@@ -4063,7 +4066,7 @@
         <v>150</v>
       </c>
       <c r="C148" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D148">
         <v>154863</v>
@@ -4080,7 +4083,7 @@
         <v>151</v>
       </c>
       <c r="C149" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D149">
         <v>159793</v>
@@ -4097,7 +4100,7 @@
         <v>152</v>
       </c>
       <c r="C150" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D150">
         <v>165455</v>
@@ -4114,7 +4117,7 @@
         <v>153</v>
       </c>
       <c r="C151" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D151">
         <v>170485</v>
@@ -4131,7 +4134,7 @@
         <v>154</v>
       </c>
       <c r="C152" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D152">
         <v>175202</v>
@@ -4148,7 +4151,7 @@
         <v>155</v>
       </c>
       <c r="C153" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D153">
         <v>180545</v>
@@ -4165,7 +4168,7 @@
         <v>156</v>
       </c>
       <c r="C154" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D154">
         <v>185122</v>
@@ -4182,7 +4185,7 @@
         <v>157</v>
       </c>
       <c r="C155" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D155">
         <v>191410</v>
@@ -4199,7 +4202,7 @@
         <v>158</v>
       </c>
       <c r="C156" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D156">
         <v>196847</v>
@@ -4216,7 +4219,7 @@
         <v>159</v>
       </c>
       <c r="C157" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D157">
         <v>202951</v>
@@ -4233,7 +4236,7 @@
         <v>160</v>
       </c>
       <c r="C158" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D158">
         <v>208392</v>
@@ -4250,7 +4253,7 @@
         <v>161</v>
       </c>
       <c r="C159" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D159">
         <v>212802</v>
@@ -4267,7 +4270,7 @@
         <v>162</v>
       </c>
       <c r="C160" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D160">
         <v>216852</v>
@@ -4284,7 +4287,7 @@
         <v>163</v>
       </c>
       <c r="C161" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D161">
         <v>220657</v>
@@ -4301,7 +4304,7 @@
         <v>164</v>
       </c>
       <c r="C162" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D162">
         <v>226089</v>
@@ -4318,7 +4321,7 @@
         <v>165</v>
       </c>
       <c r="C163" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D163">
         <v>231770</v>
@@ -4335,7 +4338,7 @@
         <v>166</v>
       </c>
       <c r="C164" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D164">
         <v>238511</v>
@@ -4352,7 +4355,7 @@
         <v>167</v>
       </c>
       <c r="C165" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D165">
         <v>245251</v>
@@ -4369,7 +4372,7 @@
         <v>168</v>
       </c>
       <c r="C166" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D166">
         <v>252165</v>
@@ -4386,7 +4389,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D167">
         <v>256848</v>
@@ -4403,7 +4406,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D168">
         <v>261750</v>
@@ -4420,7 +4423,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D169">
         <v>268008</v>
@@ -4437,7 +4440,7 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D170">
         <v>275003</v>
@@ -4454,7 +4457,7 @@
         <v>173</v>
       </c>
       <c r="C171" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D171">
         <v>282283</v>
@@ -4471,7 +4474,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D172">
         <v>289174</v>
@@ -4488,7 +4491,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D173">
         <v>295268</v>
@@ -4505,7 +4508,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D174">
         <v>299750</v>
@@ -4522,7 +4525,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D175">
         <v>304435</v>
@@ -4539,7 +4542,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D176">
         <v>311486</v>
@@ -4556,7 +4559,7 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D177">
         <v>317635</v>
@@ -4573,7 +4576,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D178">
         <v>324041</v>
@@ -4590,7 +4593,7 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D179">
         <v>331298</v>
@@ -4607,7 +4610,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D180">
         <v>338913</v>
@@ -4624,7 +4627,7 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D181">
         <v>344224</v>
@@ -4641,7 +4644,7 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D182">
         <v>349396</v>
@@ -4658,7 +4661,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D183">
         <v>356255</v>
@@ -4675,7 +4678,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D184">
         <v>362274</v>
@@ -4692,7 +4695,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D185">
         <v>370712</v>
@@ -4709,7 +4712,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D186">
         <v>378285</v>
@@ -4726,7 +4729,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D187">
         <v>385036</v>
@@ -4743,7 +4746,7 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D188">
         <v>390516</v>
@@ -4760,7 +4763,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D189">
         <v>395489</v>
@@ -4777,7 +4780,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D190">
         <v>402697</v>
@@ -4794,7 +4797,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D191">
         <v>408449</v>
@@ -4811,7 +4814,7 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D192">
         <v>416179</v>
@@ -4828,7 +4831,7 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D193">
         <v>424637</v>
@@ -4845,7 +4848,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D194">
         <v>434193</v>
@@ -4862,7 +4865,7 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D195">
         <v>439046</v>
@@ -4879,7 +4882,7 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D196">
         <v>443813</v>
@@ -4896,7 +4899,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D197">
         <v>449961</v>
@@ -4913,7 +4916,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D198">
         <v>456100</v>
@@ -4930,7 +4933,7 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D199">
         <v>462690</v>
@@ -4947,7 +4950,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D200">
         <v>469407</v>
@@ -4964,7 +4967,7 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D201">
         <v>475902</v>
@@ -4981,7 +4984,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D202">
         <v>480278</v>
@@ -4998,7 +5001,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D203">
         <v>485836</v>
@@ -5015,7 +5018,7 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D204">
         <v>492522</v>
@@ -5032,7 +5035,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D205">
         <v>498380</v>
@@ -5049,7 +5052,7 @@
         <v>208</v>
       </c>
       <c r="C206" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D206">
         <v>505751</v>
@@ -5066,7 +5069,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D207">
         <v>511369</v>
@@ -5083,7 +5086,7 @@
         <v>210</v>
       </c>
       <c r="C208" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D208">
         <v>517714</v>
@@ -5100,7 +5103,7 @@
         <v>211</v>
       </c>
       <c r="C209" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D209">
         <v>522162</v>
@@ -5117,7 +5120,7 @@
         <v>212</v>
       </c>
       <c r="C210" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D210">
         <v>525733</v>
@@ -5134,7 +5137,7 @@
         <v>213</v>
       </c>
       <c r="C211" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D211">
         <v>531239</v>
@@ -5151,7 +5154,7 @@
         <v>214</v>
       </c>
       <c r="C212" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D212">
         <v>537031</v>
@@ -5168,7 +5171,7 @@
         <v>215</v>
       </c>
       <c r="C213" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D213">
         <v>543806</v>
@@ -5185,7 +5188,7 @@
         <v>216</v>
       </c>
       <c r="C214" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D214">
         <v>549734</v>
@@ -5202,7 +5205,7 @@
         <v>217</v>
       </c>
       <c r="C215" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D215">
         <v>556216</v>
@@ -5219,7 +5222,7 @@
         <v>218</v>
       </c>
       <c r="C216" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D216">
         <v>560164</v>
@@ -5236,7 +5239,7 @@
         <v>219</v>
       </c>
       <c r="C217" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D217">
         <v>563705</v>
@@ -5253,7 +5256,7 @@
         <v>220</v>
       </c>
       <c r="C218" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D218">
         <v>568621</v>
@@ -5270,7 +5273,7 @@
         <v>221</v>
       </c>
       <c r="C219" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D219">
         <v>573888</v>
@@ -5287,7 +5290,7 @@
         <v>222</v>
       </c>
       <c r="C220" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D220">
         <v>579914</v>
@@ -5304,7 +5307,7 @@
         <v>223</v>
       </c>
       <c r="C221" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D221">
         <v>585738</v>
@@ -5321,7 +5324,7 @@
         <v>224</v>
       </c>
       <c r="C222" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D222">
         <v>591712</v>
@@ -5338,7 +5341,7 @@
         <v>225</v>
       </c>
       <c r="C223" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D223">
         <v>595841</v>
@@ -5355,7 +5358,7 @@
         <v>226</v>
       </c>
       <c r="C224" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D224">
         <v>599560</v>
@@ -5372,7 +5375,7 @@
         <v>227</v>
       </c>
       <c r="C225" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D225">
         <v>606036</v>
@@ -5389,7 +5392,7 @@
         <v>228</v>
       </c>
       <c r="C226" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D226">
         <v>610957</v>
@@ -5406,7 +5409,7 @@
         <v>229</v>
       </c>
       <c r="C227" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D227">
         <v>616894</v>
@@ -5423,7 +5426,7 @@
         <v>230</v>
       </c>
       <c r="C228" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D228">
         <v>623090</v>
@@ -5440,7 +5443,7 @@
         <v>231</v>
       </c>
       <c r="C229" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D229">
         <v>629409</v>
@@ -5457,7 +5460,7 @@
         <v>232</v>
       </c>
       <c r="C230" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D230">
         <v>634023</v>
@@ -5474,7 +5477,7 @@
         <v>233</v>
       </c>
       <c r="C231" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D231">
         <v>637509</v>
@@ -5491,7 +5494,7 @@
         <v>234</v>
       </c>
       <c r="C232" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D232">
         <v>642860</v>
@@ -5508,7 +5511,7 @@
         <v>235</v>
       </c>
       <c r="C233" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D233">
         <v>647321</v>
@@ -5525,7 +5528,7 @@
         <v>236</v>
       </c>
       <c r="C234" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D234">
         <v>652364</v>
@@ -5542,7 +5545,7 @@
         <v>237</v>
       </c>
       <c r="C235" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D235">
         <v>658299</v>
@@ -5559,7 +5562,7 @@
         <v>238</v>
       </c>
       <c r="C236" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D236">
         <v>663973</v>
@@ -5576,7 +5579,7 @@
         <v>239</v>
       </c>
       <c r="C237" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D237">
         <v>668381</v>
@@ -5593,7 +5596,7 @@
         <v>240</v>
       </c>
       <c r="C238" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D238">
         <v>671716</v>
@@ -5610,7 +5613,7 @@
         <v>241</v>
       </c>
       <c r="C239" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D239">
         <v>676487</v>
@@ -5627,7 +5630,7 @@
         <v>242</v>
       </c>
       <c r="C240" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D240">
         <v>680931</v>
@@ -5644,7 +5647,7 @@
         <v>243</v>
       </c>
       <c r="C241" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D241">
         <v>684113</v>
@@ -5661,7 +5664,7 @@
         <v>244</v>
       </c>
       <c r="C242" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D242">
         <v>688954</v>
@@ -5678,7 +5681,7 @@
         <v>245</v>
       </c>
       <c r="C243" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D243">
         <v>694121</v>
@@ -5695,7 +5698,7 @@
         <v>246</v>
       </c>
       <c r="C244" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D244">
         <v>697663</v>
@@ -5712,7 +5715,7 @@
         <v>247</v>
       </c>
       <c r="C245" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D245">
         <v>700580</v>
@@ -5729,7 +5732,7 @@
         <v>248</v>
       </c>
       <c r="C246" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D246">
         <v>705263</v>
@@ -5746,7 +5749,7 @@
         <v>249</v>
       </c>
       <c r="C247" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D247">
         <v>710049</v>
@@ -5763,7 +5766,7 @@
         <v>250</v>
       </c>
       <c r="C248" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D248">
         <v>715457</v>
@@ -5780,7 +5783,7 @@
         <v>251</v>
       </c>
       <c r="C249" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D249">
         <v>720858</v>
@@ -5797,7 +5800,7 @@
         <v>252</v>
       </c>
       <c r="C250" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D250">
         <v>726431</v>
@@ -5814,7 +5817,7 @@
         <v>253</v>
       </c>
       <c r="C251" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D251">
         <v>730317</v>
@@ -5831,7 +5834,7 @@
         <v>254</v>
       </c>
       <c r="C252" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D252">
         <v>733717</v>
@@ -5848,7 +5851,7 @@
         <v>255</v>
       </c>
       <c r="C253" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D253">
         <v>738163</v>
@@ -5865,7 +5868,7 @@
         <v>256</v>
       </c>
       <c r="C254" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D254">
         <v>743216</v>
@@ -5882,7 +5885,7 @@
         <v>257</v>
       </c>
       <c r="C255" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D255">
         <v>748315</v>
@@ -5899,7 +5902,7 @@
         <v>258</v>
       </c>
       <c r="C256" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D256">
         <v>753090</v>
@@ -5916,7 +5919,7 @@
         <v>259</v>
       </c>
       <c r="C257" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D257">
         <v>757953</v>
@@ -5933,7 +5936,7 @@
         <v>260</v>
       </c>
       <c r="C258" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D258">
         <v>761665</v>
@@ -5950,7 +5953,7 @@
         <v>261</v>
       </c>
       <c r="C259" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D259">
         <v>789780</v>
@@ -5967,7 +5970,7 @@
         <v>262</v>
       </c>
       <c r="C260" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D260">
         <v>794608</v>
@@ -5984,7 +5987,7 @@
         <v>263</v>
       </c>
       <c r="C261" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D261">
         <v>799188</v>
@@ -6001,7 +6004,7 @@
         <v>264</v>
       </c>
       <c r="C262" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D262">
         <v>804488</v>
@@ -6018,7 +6021,7 @@
         <v>265</v>
       </c>
       <c r="C263" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D263">
         <v>810020</v>
@@ -6035,7 +6038,7 @@
         <v>266</v>
       </c>
       <c r="C264" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D264">
         <v>814328</v>
@@ -6052,7 +6055,7 @@
         <v>267</v>
       </c>
       <c r="C265" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D265">
         <v>817503</v>
@@ -6069,7 +6072,7 @@
         <v>268</v>
       </c>
       <c r="C266" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D266">
         <v>821045</v>
@@ -6086,7 +6089,7 @@
         <v>269</v>
       </c>
       <c r="C267" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D267">
         <v>825340</v>
@@ -6103,7 +6106,7 @@
         <v>270</v>
       </c>
       <c r="C268" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D268">
         <v>829396</v>
@@ -6120,7 +6123,7 @@
         <v>271</v>
       </c>
       <c r="C269" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D269">
         <v>834910</v>
@@ -6137,7 +6140,7 @@
         <v>272</v>
       </c>
       <c r="C270" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D270">
         <v>841661</v>
@@ -6154,7 +6157,7 @@
         <v>273</v>
       </c>
       <c r="C271" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D271">
         <v>847108</v>
@@ -6171,7 +6174,7 @@
         <v>274</v>
       </c>
       <c r="C272" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D272">
         <v>851227</v>
@@ -6188,7 +6191,7 @@
         <v>275</v>
       </c>
       <c r="C273" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D273">
         <v>854926</v>
@@ -6205,7 +6208,7 @@
         <v>276</v>
       </c>
       <c r="C274" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D274">
         <v>860714</v>
@@ -6222,7 +6225,7 @@
         <v>277</v>
       </c>
       <c r="C275" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D275">
         <v>867559</v>
@@ -6239,7 +6242,7 @@
         <v>278</v>
       </c>
       <c r="C276" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D276">
         <v>874171</v>
@@ -6256,7 +6259,7 @@
         <v>279</v>
       </c>
       <c r="C277" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D277">
         <v>880775</v>
@@ -6273,7 +6276,7 @@
         <v>280</v>
       </c>
       <c r="C278" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D278">
         <v>886800</v>
@@ -6290,7 +6293,7 @@
         <v>281</v>
       </c>
       <c r="C279" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D279">
         <v>891160</v>
@@ -6307,7 +6310,7 @@
         <v>282</v>
       </c>
       <c r="C280" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D280">
         <v>895326</v>
@@ -6324,7 +6327,7 @@
         <v>283</v>
       </c>
       <c r="C281" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D281">
         <v>901268</v>
@@ -6341,7 +6344,7 @@
         <v>284</v>
       </c>
       <c r="C282" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D282">
         <v>906863</v>
@@ -6358,7 +6361,7 @@
         <v>285</v>
       </c>
       <c r="C283" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D283">
         <v>912811</v>
@@ -6375,7 +6378,7 @@
         <v>286</v>
       </c>
       <c r="C284" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D284">
         <v>918811</v>
@@ -6392,7 +6395,7 @@
         <v>287</v>
       </c>
       <c r="C285" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D285">
         <v>924962</v>
@@ -6409,7 +6412,7 @@
         <v>288</v>
       </c>
       <c r="C286" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D286">
         <v>929392</v>
@@ -6426,7 +6429,7 @@
         <v>289</v>
       </c>
       <c r="C287" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D287">
         <v>933155</v>
@@ -6443,7 +6446,7 @@
         <v>290</v>
       </c>
       <c r="C288" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D288">
         <v>938405</v>
@@ -6460,7 +6463,7 @@
         <v>291</v>
       </c>
       <c r="C289" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D289">
         <v>943630</v>
@@ -6477,7 +6480,7 @@
         <v>292</v>
       </c>
       <c r="C290" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D290">
         <v>949197</v>
@@ -6494,7 +6497,7 @@
         <v>293</v>
       </c>
       <c r="C291" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D291">
         <v>955128</v>
@@ -6511,7 +6514,7 @@
         <v>294</v>
       </c>
       <c r="C292" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D292">
         <v>961938</v>
@@ -6528,7 +6531,7 @@
         <v>295</v>
       </c>
       <c r="C293" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D293">
         <v>967825</v>
@@ -6545,7 +6548,7 @@
         <v>296</v>
       </c>
       <c r="C294" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D294">
         <v>972785</v>
@@ -6562,7 +6565,7 @@
         <v>297</v>
       </c>
       <c r="C295" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D295">
         <v>978531</v>
@@ -6579,7 +6582,7 @@
         <v>298</v>
       </c>
       <c r="C296" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D296">
         <v>986177</v>
@@ -6596,7 +6599,7 @@
         <v>299</v>
       </c>
       <c r="C297" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D297">
         <v>991835</v>
@@ -6613,7 +6616,7 @@
         <v>300</v>
       </c>
       <c r="C298" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D298">
         <v>997393</v>
@@ -6630,7 +6633,7 @@
         <v>301</v>
       </c>
       <c r="C299" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D299">
         <v>1003253</v>
@@ -6647,7 +6650,7 @@
         <v>302</v>
       </c>
       <c r="C300" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D300">
         <v>1006522</v>
@@ -6664,7 +6667,7 @@
         <v>303</v>
       </c>
       <c r="C301" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D301">
         <v>1009396</v>
@@ -6681,7 +6684,7 @@
         <v>304</v>
       </c>
       <c r="C302" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D302">
         <v>1011153</v>
@@ -6698,7 +6701,7 @@
         <v>305</v>
       </c>
       <c r="C303" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D303">
         <v>1015071</v>
@@ -6715,7 +6718,7 @@
         <v>306</v>
       </c>
       <c r="C304" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D304">
         <v>1019543</v>
@@ -6732,7 +6735,7 @@
         <v>307</v>
       </c>
       <c r="C305" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D305">
         <v>1025969</v>
@@ -6749,7 +6752,7 @@
         <v>308</v>
       </c>
       <c r="C306" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D306">
         <v>1032688</v>
@@ -6766,7 +6769,7 @@
         <v>309</v>
       </c>
       <c r="C307" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D307">
         <v>1041875</v>
@@ -6783,7 +6786,7 @@
         <v>310</v>
       </c>
       <c r="C308" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D308">
         <v>1049358</v>
@@ -6800,7 +6803,7 @@
         <v>311</v>
       </c>
       <c r="C309" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D309">
         <v>1060152</v>
@@ -6817,7 +6820,7 @@
         <v>312</v>
       </c>
       <c r="C310" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D310">
         <v>1070487</v>
@@ -6834,7 +6837,7 @@
         <v>313</v>
       </c>
       <c r="C311" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D311">
         <v>1078594</v>
@@ -6851,7 +6854,7 @@
         <v>314</v>
       </c>
       <c r="C312" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D312">
         <v>1090675</v>
@@ -6868,7 +6871,7 @@
         <v>315</v>
       </c>
       <c r="C313" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D313">
         <v>1101403</v>
@@ -6885,7 +6888,7 @@
         <v>316</v>
       </c>
       <c r="C314" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D314">
         <v>1107071</v>
@@ -6902,7 +6905,7 @@
         <v>317</v>
       </c>
       <c r="C315" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D315">
         <v>1113543</v>
@@ -6919,7 +6922,7 @@
         <v>318</v>
       </c>
       <c r="C316" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D316">
         <v>1122362</v>
@@ -6936,7 +6939,7 @@
         <v>319</v>
       </c>
       <c r="C317" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D317">
         <v>1133613</v>
@@ -6953,7 +6956,7 @@
         <v>320</v>
       </c>
       <c r="C318" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D318">
         <v>1144643</v>
@@ -6970,7 +6973,7 @@
         <v>321</v>
       </c>
       <c r="C319" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D319">
         <v>1156770</v>
@@ -6987,7 +6990,7 @@
         <v>322</v>
       </c>
       <c r="C320" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D320">
         <v>1168395</v>
@@ -7004,7 +7007,7 @@
         <v>323</v>
       </c>
       <c r="C321" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D321">
         <v>1175850</v>
@@ -7021,7 +7024,7 @@
         <v>324</v>
       </c>
       <c r="C322" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D322">
         <v>1182249</v>
@@ -7038,7 +7041,7 @@
         <v>325</v>
       </c>
       <c r="C323" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D323">
         <v>1193255</v>
@@ -7055,7 +7058,7 @@
         <v>326</v>
       </c>
       <c r="C324" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D324">
         <v>1205229</v>
@@ -7072,7 +7075,7 @@
         <v>327</v>
       </c>
       <c r="C325" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D325">
         <v>1217126</v>
@@ -7089,7 +7092,7 @@
         <v>328</v>
       </c>
       <c r="C326" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D326">
         <v>1229379</v>
@@ -7106,7 +7109,7 @@
         <v>329</v>
       </c>
       <c r="C327" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D327">
         <v>1241436</v>
@@ -7123,7 +7126,7 @@
         <v>330</v>
       </c>
       <c r="C328" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D328">
         <v>1250044</v>
@@ -7140,7 +7143,7 @@
         <v>331</v>
       </c>
       <c r="C329" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D329">
         <v>1255974</v>
@@ -7157,7 +7160,7 @@
         <v>332</v>
       </c>
       <c r="C330" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D330">
         <v>1267202</v>
@@ -7174,7 +7177,7 @@
         <v>333</v>
       </c>
       <c r="C331" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D331">
         <v>1277499</v>
@@ -7191,7 +7194,7 @@
         <v>334</v>
       </c>
       <c r="C332" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D332">
         <v>1289298</v>
@@ -7208,7 +7211,7 @@
         <v>335</v>
       </c>
       <c r="C333" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D333">
         <v>1301546</v>
@@ -7225,7 +7228,7 @@
         <v>336</v>
       </c>
       <c r="C334" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D334">
         <v>1313675</v>
@@ -7242,7 +7245,7 @@
         <v>337</v>
       </c>
       <c r="C335" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D335">
         <v>1320545</v>
@@ -7259,7 +7262,7 @@
         <v>338</v>
       </c>
       <c r="C336" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D336">
         <v>1325915</v>
@@ -7276,7 +7279,7 @@
         <v>339</v>
       </c>
       <c r="C337" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D337">
         <v>1338426</v>
@@ -7293,7 +7296,7 @@
         <v>340</v>
       </c>
       <c r="C338" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D338">
         <v>1350079</v>
@@ -7310,7 +7313,7 @@
         <v>341</v>
       </c>
       <c r="C339" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D339">
         <v>1362564</v>
@@ -7327,7 +7330,7 @@
         <v>342</v>
       </c>
       <c r="C340" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D340">
         <v>1372243</v>
@@ -7344,7 +7347,7 @@
         <v>343</v>
       </c>
       <c r="C341" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D341">
         <v>1377217</v>
@@ -7361,7 +7364,7 @@
         <v>344</v>
       </c>
       <c r="C342" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D342">
         <v>1383434</v>
@@ -7378,7 +7381,7 @@
         <v>345</v>
       </c>
       <c r="C343" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D343">
         <v>1389430</v>
@@ -7395,7 +7398,7 @@
         <v>346</v>
       </c>
       <c r="C344" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D344">
         <v>1401529</v>
@@ -7412,7 +7415,7 @@
         <v>347</v>
       </c>
       <c r="C345" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D345">
         <v>1413935</v>
@@ -7429,7 +7432,7 @@
         <v>348</v>
       </c>
       <c r="C346" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D346">
         <v>1426094</v>
@@ -7446,7 +7449,7 @@
         <v>349</v>
       </c>
       <c r="C347" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D347">
         <v>1437185</v>
@@ -7463,7 +7466,7 @@
         <v>350</v>
       </c>
       <c r="C348" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D348">
         <v>1443544</v>
@@ -7480,7 +7483,7 @@
         <v>351</v>
       </c>
       <c r="C349" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D349">
         <v>1448755</v>
@@ -7497,7 +7500,7 @@
         <v>352</v>
       </c>
       <c r="C350" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D350">
         <v>1455219</v>
@@ -7514,7 +7517,7 @@
         <v>353</v>
       </c>
       <c r="C351" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D351">
         <v>1466490</v>
@@ -7531,7 +7534,7 @@
         <v>354</v>
       </c>
       <c r="C352" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D352">
         <v>1479835</v>
@@ -7548,7 +7551,7 @@
         <v>355</v>
       </c>
       <c r="C353" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D353">
         <v>1493569</v>
@@ -7565,7 +7568,7 @@
         <v>356</v>
       </c>
       <c r="C354" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D354">
         <v>1507931</v>
@@ -7582,7 +7585,7 @@
         <v>357</v>
       </c>
       <c r="C355" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D355">
         <v>1524036</v>
@@ -7599,7 +7602,7 @@
         <v>358</v>
       </c>
       <c r="C356" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D356">
         <v>1534039</v>
@@ -7616,7 +7619,7 @@
         <v>359</v>
       </c>
       <c r="C357" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D357">
         <v>1541633</v>
@@ -7633,7 +7636,7 @@
         <v>360</v>
       </c>
       <c r="C358" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D358">
         <v>1556028</v>
@@ -7650,7 +7653,7 @@
         <v>361</v>
       </c>
       <c r="C359" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D359">
         <v>1571901</v>
@@ -7667,7 +7670,7 @@
         <v>362</v>
       </c>
       <c r="C360" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D360">
         <v>1588369</v>
@@ -7684,7 +7687,7 @@
         <v>363</v>
       </c>
       <c r="C361" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D361">
         <v>1609735</v>
@@ -7701,7 +7704,7 @@
         <v>364</v>
       </c>
       <c r="C362" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D362">
         <v>1630258</v>
@@ -7718,7 +7721,7 @@
         <v>365</v>
       </c>
       <c r="C363" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D363">
         <v>1641428</v>
@@ -7735,7 +7738,7 @@
         <v>366</v>
       </c>
       <c r="C364" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D364">
         <v>1649502</v>
@@ -7752,7 +7755,7 @@
         <v>367</v>
       </c>
       <c r="C365" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D365">
         <v>1668396</v>
@@ -7769,7 +7772,7 @@
         <v>368</v>
       </c>
       <c r="C366" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D366">
         <v>1688944</v>
@@ -7786,7 +7789,7 @@
         <v>369</v>
       </c>
       <c r="C367" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D367">
         <v>1711283</v>
@@ -7803,7 +7806,7 @@
         <v>370</v>
       </c>
       <c r="C368" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D368">
         <v>1732290</v>
@@ -7820,7 +7823,7 @@
         <v>371</v>
       </c>
       <c r="C369" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D369">
         <v>1752347</v>
@@ -7837,7 +7840,7 @@
         <v>372</v>
       </c>
       <c r="C370" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D370">
         <v>1763219</v>
@@ -7854,7 +7857,7 @@
         <v>373</v>
       </c>
       <c r="C371" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D371">
         <v>1771740</v>
@@ -7871,7 +7874,7 @@
         <v>374</v>
       </c>
       <c r="C372" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D372">
         <v>1788905</v>
@@ -7888,7 +7891,7 @@
         <v>375</v>
       </c>
       <c r="C373" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D373">
         <v>1806849</v>
@@ -7905,7 +7908,7 @@
         <v>376</v>
       </c>
       <c r="C374" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D374">
         <v>1825519</v>
@@ -7922,7 +7925,7 @@
         <v>377</v>
       </c>
       <c r="C375" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D375">
         <v>1841893</v>
@@ -7939,7 +7942,7 @@
         <v>378</v>
       </c>
       <c r="C376" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D376">
         <v>1857230</v>
@@ -7956,7 +7959,7 @@
         <v>379</v>
       </c>
       <c r="C377" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D377">
         <v>1864260</v>
@@ -7973,7 +7976,7 @@
         <v>380</v>
       </c>
       <c r="C378" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D378">
         <v>1869708</v>
@@ -7990,7 +7993,7 @@
         <v>381</v>
       </c>
       <c r="C379" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D379">
         <v>1874092</v>
@@ -8007,7 +8010,7 @@
         <v>382</v>
       </c>
       <c r="C380" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D380">
         <v>1886245</v>
@@ -8024,7 +8027,7 @@
         <v>383</v>
       </c>
       <c r="C381" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D381">
         <v>1886245</v>
@@ -8041,7 +8044,7 @@
         <v>384</v>
       </c>
       <c r="C382" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D382">
         <v>1912871</v>
@@ -8058,7 +8061,7 @@
         <v>385</v>
       </c>
       <c r="C383" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D383">
         <v>1926080</v>
@@ -8075,7 +8078,7 @@
         <v>386</v>
       </c>
       <c r="C384" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D384">
         <v>1932145</v>
@@ -8092,7 +8095,7 @@
         <v>387</v>
       </c>
       <c r="C385" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D385">
         <v>1936013</v>
@@ -8109,7 +8112,7 @@
         <v>388</v>
       </c>
       <c r="C386" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D386">
         <v>1946751</v>
@@ -8126,7 +8129,7 @@
         <v>389</v>
       </c>
       <c r="C387" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D387">
         <v>1957889</v>
@@ -8143,7 +8146,7 @@
         <v>390</v>
       </c>
       <c r="C388" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D388">
         <v>1968566</v>
@@ -8160,7 +8163,7 @@
         <v>391</v>
       </c>
       <c r="C389" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D389">
         <v>1978954</v>
@@ -8177,13 +8180,30 @@
         <v>392</v>
       </c>
       <c r="C390" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D390">
         <v>1988695</v>
       </c>
       <c r="E390">
         <v>173771</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5">
+      <c r="A391" s="1">
+        <v>389</v>
+      </c>
+      <c r="B391" t="s">
+        <v>393</v>
+      </c>
+      <c r="C391" t="s">
+        <v>394</v>
+      </c>
+      <c r="D391">
+        <v>1992794</v>
+      </c>
+      <c r="E391">
+        <v>174207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subdivided per month and ploted
</commit_message>
<xml_diff>
--- a/mexico.xlsx
+++ b/mexico.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="395">
   <si>
     <t>date</t>
   </si>
@@ -1193,6 +1193,9 @@
   </si>
   <si>
     <t>2021-02-13</t>
+  </si>
+  <si>
+    <t>2021-02-14</t>
   </si>
   <si>
     <t>mexico</t>
@@ -1553,7 +1556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E390"/>
+  <dimension ref="A1:E391"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1581,7 +1584,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1598,7 +1601,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1615,7 +1618,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1632,7 +1635,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1649,7 +1652,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1666,7 +1669,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1683,7 +1686,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1700,7 +1703,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1717,7 +1720,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1734,7 +1737,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1751,7 +1754,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1768,7 +1771,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1785,7 +1788,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1802,7 +1805,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1819,7 +1822,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1836,7 +1839,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1853,7 +1856,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1870,7 +1873,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1887,7 +1890,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1904,7 +1907,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1921,7 +1924,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1938,7 +1941,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1955,7 +1958,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1972,7 +1975,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1989,7 +1992,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2006,7 +2009,7 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2023,7 +2026,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2040,7 +2043,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2057,7 +2060,7 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2074,7 +2077,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2091,7 +2094,7 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2108,7 +2111,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2125,7 +2128,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2142,7 +2145,7 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2159,7 +2162,7 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2176,7 +2179,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2193,7 +2196,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2210,7 +2213,7 @@
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2227,7 +2230,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -2244,7 +2247,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D41">
         <v>5</v>
@@ -2261,7 +2264,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D42">
         <v>5</v>
@@ -2278,7 +2281,7 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2295,7 +2298,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D44">
         <v>5</v>
@@ -2312,7 +2315,7 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D45">
         <v>5</v>
@@ -2329,7 +2332,7 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D46">
         <v>6</v>
@@ -2346,7 +2349,7 @@
         <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D47">
         <v>6</v>
@@ -2363,7 +2366,7 @@
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D48">
         <v>7</v>
@@ -2380,7 +2383,7 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D49">
         <v>7</v>
@@ -2397,7 +2400,7 @@
         <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D50">
         <v>7</v>
@@ -2414,7 +2417,7 @@
         <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D51">
         <v>8</v>
@@ -2431,7 +2434,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D52">
         <v>12</v>
@@ -2448,7 +2451,7 @@
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D53">
         <v>26</v>
@@ -2465,7 +2468,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D54">
         <v>41</v>
@@ -2482,7 +2485,7 @@
         <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D55">
         <v>53</v>
@@ -2499,7 +2502,7 @@
         <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D56">
         <v>82</v>
@@ -2516,7 +2519,7 @@
         <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D57">
         <v>93</v>
@@ -2533,7 +2536,7 @@
         <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D58">
         <v>118</v>
@@ -2550,7 +2553,7 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D59">
         <v>164</v>
@@ -2567,7 +2570,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D60">
         <v>203</v>
@@ -2584,7 +2587,7 @@
         <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D61">
         <v>251</v>
@@ -2601,7 +2604,7 @@
         <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D62">
         <v>316</v>
@@ -2618,7 +2621,7 @@
         <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D63">
         <v>367</v>
@@ -2635,7 +2638,7 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D64">
         <v>405</v>
@@ -2652,7 +2655,7 @@
         <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D65">
         <v>475</v>
@@ -2669,7 +2672,7 @@
         <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D66">
         <v>585</v>
@@ -2686,7 +2689,7 @@
         <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D67">
         <v>717</v>
@@ -2703,7 +2706,7 @@
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D68">
         <v>848</v>
@@ -2720,7 +2723,7 @@
         <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D69">
         <v>993</v>
@@ -2737,7 +2740,7 @@
         <v>72</v>
       </c>
       <c r="C70" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D70">
         <v>1094</v>
@@ -2754,7 +2757,7 @@
         <v>73</v>
       </c>
       <c r="C71" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D71">
         <v>1215</v>
@@ -2771,7 +2774,7 @@
         <v>74</v>
       </c>
       <c r="C72" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D72">
         <v>1378</v>
@@ -2788,7 +2791,7 @@
         <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D73">
         <v>1510</v>
@@ -2805,7 +2808,7 @@
         <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D74">
         <v>1688</v>
@@ -2822,7 +2825,7 @@
         <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D75">
         <v>1890</v>
@@ -2839,7 +2842,7 @@
         <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D76">
         <v>2143</v>
@@ -2856,7 +2859,7 @@
         <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D77">
         <v>2439</v>
@@ -2873,7 +2876,7 @@
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D78">
         <v>2785</v>
@@ -2890,7 +2893,7 @@
         <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D79">
         <v>3181</v>
@@ -2907,7 +2910,7 @@
         <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D80">
         <v>3441</v>
@@ -2924,7 +2927,7 @@
         <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D81">
         <v>3844</v>
@@ -2941,7 +2944,7 @@
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D82">
         <v>4219</v>
@@ -2958,7 +2961,7 @@
         <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D83">
         <v>4661</v>
@@ -2975,7 +2978,7 @@
         <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D84">
         <v>5014</v>
@@ -2992,7 +2995,7 @@
         <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D85">
         <v>5399</v>
@@ -3009,7 +3012,7 @@
         <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D86">
         <v>5847</v>
@@ -3026,7 +3029,7 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D87">
         <v>6297</v>
@@ -3043,7 +3046,7 @@
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D88">
         <v>6875</v>
@@ -3060,7 +3063,7 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D89">
         <v>7497</v>
@@ -3077,7 +3080,7 @@
         <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D90">
         <v>8261</v>
@@ -3094,7 +3097,7 @@
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D91">
         <v>8772</v>
@@ -3111,7 +3114,7 @@
         <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D92">
         <v>9501</v>
@@ -3128,7 +3131,7 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D93">
         <v>10544</v>
@@ -3145,7 +3148,7 @@
         <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D94">
         <v>11633</v>
@@ -3162,7 +3165,7 @@
         <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D95">
         <v>12872</v>
@@ -3179,7 +3182,7 @@
         <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D96">
         <v>13842</v>
@@ -3196,7 +3199,7 @@
         <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D97">
         <v>14677</v>
@@ -3213,7 +3216,7 @@
         <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D98">
         <v>15529</v>
@@ -3230,7 +3233,7 @@
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D99">
         <v>16752</v>
@@ -3247,7 +3250,7 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D100">
         <v>17799</v>
@@ -3264,7 +3267,7 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D101">
         <v>19224</v>
@@ -3281,7 +3284,7 @@
         <v>104</v>
       </c>
       <c r="C102" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D102">
         <v>20739</v>
@@ -3298,7 +3301,7 @@
         <v>105</v>
       </c>
       <c r="C103" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D103">
         <v>22088</v>
@@ -3315,7 +3318,7 @@
         <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D104">
         <v>23471</v>
@@ -3332,7 +3335,7 @@
         <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D105">
         <v>24905</v>
@@ -3349,7 +3352,7 @@
         <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D106">
         <v>26025</v>
@@ -3366,7 +3369,7 @@
         <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D107">
         <v>27634</v>
@@ -3383,7 +3386,7 @@
         <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D108">
         <v>29616</v>
@@ -3400,7 +3403,7 @@
         <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D109">
         <v>31522</v>
@@ -3417,7 +3420,7 @@
         <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D110">
         <v>33460</v>
@@ -3434,7 +3437,7 @@
         <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D111">
         <v>35022</v>
@@ -3451,7 +3454,7 @@
         <v>114</v>
       </c>
       <c r="C112" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D112">
         <v>36327</v>
@@ -3468,7 +3471,7 @@
         <v>115</v>
       </c>
       <c r="C113" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D113">
         <v>38324</v>
@@ -3485,7 +3488,7 @@
         <v>116</v>
       </c>
       <c r="C114" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D114">
         <v>40186</v>
@@ -3502,7 +3505,7 @@
         <v>117</v>
       </c>
       <c r="C115" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D115">
         <v>42595</v>
@@ -3519,7 +3522,7 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D116">
         <v>45032</v>
@@ -3536,7 +3539,7 @@
         <v>119</v>
       </c>
       <c r="C117" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D117">
         <v>47144</v>
@@ -3553,7 +3556,7 @@
         <v>120</v>
       </c>
       <c r="C118" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D118">
         <v>49219</v>
@@ -3570,7 +3573,7 @@
         <v>121</v>
       </c>
       <c r="C119" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D119">
         <v>51633</v>
@@ -3587,7 +3590,7 @@
         <v>122</v>
       </c>
       <c r="C120" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D120">
         <v>54346</v>
@@ -3604,7 +3607,7 @@
         <v>123</v>
       </c>
       <c r="C121" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D121">
         <v>56594</v>
@@ -3621,7 +3624,7 @@
         <v>124</v>
       </c>
       <c r="C122" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D122">
         <v>59567</v>
@@ -3638,7 +3641,7 @@
         <v>125</v>
       </c>
       <c r="C123" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D123">
         <v>62527</v>
@@ -3655,7 +3658,7 @@
         <v>126</v>
       </c>
       <c r="C124" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D124">
         <v>65856</v>
@@ -3672,7 +3675,7 @@
         <v>127</v>
       </c>
       <c r="C125" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D125">
         <v>68620</v>
@@ -3689,7 +3692,7 @@
         <v>128</v>
       </c>
       <c r="C126" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D126">
         <v>71105</v>
@@ -3706,7 +3709,7 @@
         <v>129</v>
       </c>
       <c r="C127" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D127">
         <v>74560</v>
@@ -3723,7 +3726,7 @@
         <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D128">
         <v>78023</v>
@@ -3740,7 +3743,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D129">
         <v>81400</v>
@@ -3757,7 +3760,7 @@
         <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D130">
         <v>84627</v>
@@ -3774,7 +3777,7 @@
         <v>133</v>
       </c>
       <c r="C131" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D131">
         <v>87512</v>
@@ -3791,7 +3794,7 @@
         <v>134</v>
       </c>
       <c r="C132" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D132">
         <v>90664</v>
@@ -3808,7 +3811,7 @@
         <v>135</v>
       </c>
       <c r="C133" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D133">
         <v>93435</v>
@@ -3825,7 +3828,7 @@
         <v>136</v>
       </c>
       <c r="C134" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D134">
         <v>97326</v>
@@ -3842,7 +3845,7 @@
         <v>137</v>
       </c>
       <c r="C135" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D135">
         <v>101238</v>
@@ -3859,7 +3862,7 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D136">
         <v>105680</v>
@@ -3876,7 +3879,7 @@
         <v>139</v>
       </c>
       <c r="C137" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D137">
         <v>110026</v>
@@ -3893,7 +3896,7 @@
         <v>140</v>
       </c>
       <c r="C138" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D138">
         <v>113619</v>
@@ -3910,7 +3913,7 @@
         <v>141</v>
       </c>
       <c r="C139" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D139">
         <v>117103</v>
@@ -3927,7 +3930,7 @@
         <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D140">
         <v>120102</v>
@@ -3944,7 +3947,7 @@
         <v>143</v>
       </c>
       <c r="C141" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D141">
         <v>124301</v>
@@ -3961,7 +3964,7 @@
         <v>144</v>
       </c>
       <c r="C142" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D142">
         <v>129184</v>
@@ -3978,7 +3981,7 @@
         <v>145</v>
       </c>
       <c r="C143" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D143">
         <v>133974</v>
@@ -3995,7 +3998,7 @@
         <v>146</v>
       </c>
       <c r="C144" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D144">
         <v>139196</v>
@@ -4012,7 +4015,7 @@
         <v>147</v>
       </c>
       <c r="C145" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D145">
         <v>142690</v>
@@ -4029,7 +4032,7 @@
         <v>148</v>
       </c>
       <c r="C146" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D146">
         <v>146837</v>
@@ -4046,7 +4049,7 @@
         <v>149</v>
       </c>
       <c r="C147" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D147">
         <v>150264</v>
@@ -4063,7 +4066,7 @@
         <v>150</v>
       </c>
       <c r="C148" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D148">
         <v>154863</v>
@@ -4080,7 +4083,7 @@
         <v>151</v>
       </c>
       <c r="C149" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D149">
         <v>159793</v>
@@ -4097,7 +4100,7 @@
         <v>152</v>
       </c>
       <c r="C150" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D150">
         <v>165455</v>
@@ -4114,7 +4117,7 @@
         <v>153</v>
       </c>
       <c r="C151" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D151">
         <v>170485</v>
@@ -4131,7 +4134,7 @@
         <v>154</v>
       </c>
       <c r="C152" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D152">
         <v>175202</v>
@@ -4148,7 +4151,7 @@
         <v>155</v>
       </c>
       <c r="C153" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D153">
         <v>180545</v>
@@ -4165,7 +4168,7 @@
         <v>156</v>
       </c>
       <c r="C154" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D154">
         <v>185122</v>
@@ -4182,7 +4185,7 @@
         <v>157</v>
       </c>
       <c r="C155" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D155">
         <v>191410</v>
@@ -4199,7 +4202,7 @@
         <v>158</v>
       </c>
       <c r="C156" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D156">
         <v>196847</v>
@@ -4216,7 +4219,7 @@
         <v>159</v>
       </c>
       <c r="C157" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D157">
         <v>202951</v>
@@ -4233,7 +4236,7 @@
         <v>160</v>
       </c>
       <c r="C158" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D158">
         <v>208392</v>
@@ -4250,7 +4253,7 @@
         <v>161</v>
       </c>
       <c r="C159" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D159">
         <v>212802</v>
@@ -4267,7 +4270,7 @@
         <v>162</v>
       </c>
       <c r="C160" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D160">
         <v>216852</v>
@@ -4284,7 +4287,7 @@
         <v>163</v>
       </c>
       <c r="C161" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D161">
         <v>220657</v>
@@ -4301,7 +4304,7 @@
         <v>164</v>
       </c>
       <c r="C162" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D162">
         <v>226089</v>
@@ -4318,7 +4321,7 @@
         <v>165</v>
       </c>
       <c r="C163" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D163">
         <v>231770</v>
@@ -4335,7 +4338,7 @@
         <v>166</v>
       </c>
       <c r="C164" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D164">
         <v>238511</v>
@@ -4352,7 +4355,7 @@
         <v>167</v>
       </c>
       <c r="C165" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D165">
         <v>245251</v>
@@ -4369,7 +4372,7 @@
         <v>168</v>
       </c>
       <c r="C166" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D166">
         <v>252165</v>
@@ -4386,7 +4389,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D167">
         <v>256848</v>
@@ -4403,7 +4406,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D168">
         <v>261750</v>
@@ -4420,7 +4423,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D169">
         <v>268008</v>
@@ -4437,7 +4440,7 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D170">
         <v>275003</v>
@@ -4454,7 +4457,7 @@
         <v>173</v>
       </c>
       <c r="C171" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D171">
         <v>282283</v>
@@ -4471,7 +4474,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D172">
         <v>289174</v>
@@ -4488,7 +4491,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D173">
         <v>295268</v>
@@ -4505,7 +4508,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D174">
         <v>299750</v>
@@ -4522,7 +4525,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D175">
         <v>304435</v>
@@ -4539,7 +4542,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D176">
         <v>311486</v>
@@ -4556,7 +4559,7 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D177">
         <v>317635</v>
@@ -4573,7 +4576,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D178">
         <v>324041</v>
@@ -4590,7 +4593,7 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D179">
         <v>331298</v>
@@ -4607,7 +4610,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D180">
         <v>338913</v>
@@ -4624,7 +4627,7 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D181">
         <v>344224</v>
@@ -4641,7 +4644,7 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D182">
         <v>349396</v>
@@ -4658,7 +4661,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D183">
         <v>356255</v>
@@ -4675,7 +4678,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D184">
         <v>362274</v>
@@ -4692,7 +4695,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D185">
         <v>370712</v>
@@ -4709,7 +4712,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D186">
         <v>378285</v>
@@ -4726,7 +4729,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D187">
         <v>385036</v>
@@ -4743,7 +4746,7 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D188">
         <v>390516</v>
@@ -4760,7 +4763,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D189">
         <v>395489</v>
@@ -4777,7 +4780,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D190">
         <v>402697</v>
@@ -4794,7 +4797,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D191">
         <v>408449</v>
@@ -4811,7 +4814,7 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D192">
         <v>416179</v>
@@ -4828,7 +4831,7 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D193">
         <v>424637</v>
@@ -4845,7 +4848,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D194">
         <v>434193</v>
@@ -4862,7 +4865,7 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D195">
         <v>439046</v>
@@ -4879,7 +4882,7 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D196">
         <v>443813</v>
@@ -4896,7 +4899,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D197">
         <v>449961</v>
@@ -4913,7 +4916,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D198">
         <v>456100</v>
@@ -4930,7 +4933,7 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D199">
         <v>462690</v>
@@ -4947,7 +4950,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D200">
         <v>469407</v>
@@ -4964,7 +4967,7 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D201">
         <v>475902</v>
@@ -4981,7 +4984,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D202">
         <v>480278</v>
@@ -4998,7 +5001,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D203">
         <v>485836</v>
@@ -5015,7 +5018,7 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D204">
         <v>492522</v>
@@ -5032,7 +5035,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D205">
         <v>498380</v>
@@ -5049,7 +5052,7 @@
         <v>208</v>
       </c>
       <c r="C206" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D206">
         <v>505751</v>
@@ -5066,7 +5069,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D207">
         <v>511369</v>
@@ -5083,7 +5086,7 @@
         <v>210</v>
       </c>
       <c r="C208" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D208">
         <v>517714</v>
@@ -5100,7 +5103,7 @@
         <v>211</v>
       </c>
       <c r="C209" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D209">
         <v>522162</v>
@@ -5117,7 +5120,7 @@
         <v>212</v>
       </c>
       <c r="C210" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D210">
         <v>525733</v>
@@ -5134,7 +5137,7 @@
         <v>213</v>
       </c>
       <c r="C211" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D211">
         <v>531239</v>
@@ -5151,7 +5154,7 @@
         <v>214</v>
       </c>
       <c r="C212" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D212">
         <v>537031</v>
@@ -5168,7 +5171,7 @@
         <v>215</v>
       </c>
       <c r="C213" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D213">
         <v>543806</v>
@@ -5185,7 +5188,7 @@
         <v>216</v>
       </c>
       <c r="C214" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D214">
         <v>549734</v>
@@ -5202,7 +5205,7 @@
         <v>217</v>
       </c>
       <c r="C215" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D215">
         <v>556216</v>
@@ -5219,7 +5222,7 @@
         <v>218</v>
       </c>
       <c r="C216" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D216">
         <v>560164</v>
@@ -5236,7 +5239,7 @@
         <v>219</v>
       </c>
       <c r="C217" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D217">
         <v>563705</v>
@@ -5253,7 +5256,7 @@
         <v>220</v>
       </c>
       <c r="C218" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D218">
         <v>568621</v>
@@ -5270,7 +5273,7 @@
         <v>221</v>
       </c>
       <c r="C219" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D219">
         <v>573888</v>
@@ -5287,7 +5290,7 @@
         <v>222</v>
       </c>
       <c r="C220" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D220">
         <v>579914</v>
@@ -5304,7 +5307,7 @@
         <v>223</v>
       </c>
       <c r="C221" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D221">
         <v>585738</v>
@@ -5321,7 +5324,7 @@
         <v>224</v>
       </c>
       <c r="C222" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D222">
         <v>591712</v>
@@ -5338,7 +5341,7 @@
         <v>225</v>
       </c>
       <c r="C223" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D223">
         <v>595841</v>
@@ -5355,7 +5358,7 @@
         <v>226</v>
       </c>
       <c r="C224" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D224">
         <v>599560</v>
@@ -5372,7 +5375,7 @@
         <v>227</v>
       </c>
       <c r="C225" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D225">
         <v>606036</v>
@@ -5389,7 +5392,7 @@
         <v>228</v>
       </c>
       <c r="C226" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D226">
         <v>610957</v>
@@ -5406,7 +5409,7 @@
         <v>229</v>
       </c>
       <c r="C227" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D227">
         <v>616894</v>
@@ -5423,7 +5426,7 @@
         <v>230</v>
       </c>
       <c r="C228" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D228">
         <v>623090</v>
@@ -5440,7 +5443,7 @@
         <v>231</v>
       </c>
       <c r="C229" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D229">
         <v>629409</v>
@@ -5457,7 +5460,7 @@
         <v>232</v>
       </c>
       <c r="C230" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D230">
         <v>634023</v>
@@ -5474,7 +5477,7 @@
         <v>233</v>
       </c>
       <c r="C231" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D231">
         <v>637509</v>
@@ -5491,7 +5494,7 @@
         <v>234</v>
       </c>
       <c r="C232" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D232">
         <v>642860</v>
@@ -5508,7 +5511,7 @@
         <v>235</v>
       </c>
       <c r="C233" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D233">
         <v>647321</v>
@@ -5525,7 +5528,7 @@
         <v>236</v>
       </c>
       <c r="C234" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D234">
         <v>652364</v>
@@ -5542,7 +5545,7 @@
         <v>237</v>
       </c>
       <c r="C235" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D235">
         <v>658299</v>
@@ -5559,7 +5562,7 @@
         <v>238</v>
       </c>
       <c r="C236" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D236">
         <v>663973</v>
@@ -5576,7 +5579,7 @@
         <v>239</v>
       </c>
       <c r="C237" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D237">
         <v>668381</v>
@@ -5593,7 +5596,7 @@
         <v>240</v>
       </c>
       <c r="C238" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D238">
         <v>671716</v>
@@ -5610,7 +5613,7 @@
         <v>241</v>
       </c>
       <c r="C239" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D239">
         <v>676487</v>
@@ -5627,7 +5630,7 @@
         <v>242</v>
       </c>
       <c r="C240" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D240">
         <v>680931</v>
@@ -5644,7 +5647,7 @@
         <v>243</v>
       </c>
       <c r="C241" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D241">
         <v>684113</v>
@@ -5661,7 +5664,7 @@
         <v>244</v>
       </c>
       <c r="C242" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D242">
         <v>688954</v>
@@ -5678,7 +5681,7 @@
         <v>245</v>
       </c>
       <c r="C243" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D243">
         <v>694121</v>
@@ -5695,7 +5698,7 @@
         <v>246</v>
       </c>
       <c r="C244" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D244">
         <v>697663</v>
@@ -5712,7 +5715,7 @@
         <v>247</v>
       </c>
       <c r="C245" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D245">
         <v>700580</v>
@@ -5729,7 +5732,7 @@
         <v>248</v>
       </c>
       <c r="C246" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D246">
         <v>705263</v>
@@ -5746,7 +5749,7 @@
         <v>249</v>
       </c>
       <c r="C247" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D247">
         <v>710049</v>
@@ -5763,7 +5766,7 @@
         <v>250</v>
       </c>
       <c r="C248" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D248">
         <v>715457</v>
@@ -5780,7 +5783,7 @@
         <v>251</v>
       </c>
       <c r="C249" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D249">
         <v>720858</v>
@@ -5797,7 +5800,7 @@
         <v>252</v>
       </c>
       <c r="C250" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D250">
         <v>726431</v>
@@ -5814,7 +5817,7 @@
         <v>253</v>
       </c>
       <c r="C251" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D251">
         <v>730317</v>
@@ -5831,7 +5834,7 @@
         <v>254</v>
       </c>
       <c r="C252" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D252">
         <v>733717</v>
@@ -5848,7 +5851,7 @@
         <v>255</v>
       </c>
       <c r="C253" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D253">
         <v>738163</v>
@@ -5865,7 +5868,7 @@
         <v>256</v>
       </c>
       <c r="C254" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D254">
         <v>743216</v>
@@ -5882,7 +5885,7 @@
         <v>257</v>
       </c>
       <c r="C255" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D255">
         <v>748315</v>
@@ -5899,7 +5902,7 @@
         <v>258</v>
       </c>
       <c r="C256" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D256">
         <v>753090</v>
@@ -5916,7 +5919,7 @@
         <v>259</v>
       </c>
       <c r="C257" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D257">
         <v>757953</v>
@@ -5933,7 +5936,7 @@
         <v>260</v>
       </c>
       <c r="C258" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D258">
         <v>761665</v>
@@ -5950,7 +5953,7 @@
         <v>261</v>
       </c>
       <c r="C259" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D259">
         <v>789780</v>
@@ -5967,7 +5970,7 @@
         <v>262</v>
       </c>
       <c r="C260" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D260">
         <v>794608</v>
@@ -5984,7 +5987,7 @@
         <v>263</v>
       </c>
       <c r="C261" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D261">
         <v>799188</v>
@@ -6001,7 +6004,7 @@
         <v>264</v>
       </c>
       <c r="C262" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D262">
         <v>804488</v>
@@ -6018,7 +6021,7 @@
         <v>265</v>
       </c>
       <c r="C263" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D263">
         <v>810020</v>
@@ -6035,7 +6038,7 @@
         <v>266</v>
       </c>
       <c r="C264" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D264">
         <v>814328</v>
@@ -6052,7 +6055,7 @@
         <v>267</v>
       </c>
       <c r="C265" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D265">
         <v>817503</v>
@@ -6069,7 +6072,7 @@
         <v>268</v>
       </c>
       <c r="C266" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D266">
         <v>821045</v>
@@ -6086,7 +6089,7 @@
         <v>269</v>
       </c>
       <c r="C267" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D267">
         <v>825340</v>
@@ -6103,7 +6106,7 @@
         <v>270</v>
       </c>
       <c r="C268" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D268">
         <v>829396</v>
@@ -6120,7 +6123,7 @@
         <v>271</v>
       </c>
       <c r="C269" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D269">
         <v>834910</v>
@@ -6137,7 +6140,7 @@
         <v>272</v>
       </c>
       <c r="C270" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D270">
         <v>841661</v>
@@ -6154,7 +6157,7 @@
         <v>273</v>
       </c>
       <c r="C271" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D271">
         <v>847108</v>
@@ -6171,7 +6174,7 @@
         <v>274</v>
       </c>
       <c r="C272" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D272">
         <v>851227</v>
@@ -6188,7 +6191,7 @@
         <v>275</v>
       </c>
       <c r="C273" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D273">
         <v>854926</v>
@@ -6205,7 +6208,7 @@
         <v>276</v>
       </c>
       <c r="C274" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D274">
         <v>860714</v>
@@ -6222,7 +6225,7 @@
         <v>277</v>
       </c>
       <c r="C275" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D275">
         <v>867559</v>
@@ -6239,7 +6242,7 @@
         <v>278</v>
       </c>
       <c r="C276" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D276">
         <v>874171</v>
@@ -6256,7 +6259,7 @@
         <v>279</v>
       </c>
       <c r="C277" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D277">
         <v>880775</v>
@@ -6273,7 +6276,7 @@
         <v>280</v>
       </c>
       <c r="C278" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D278">
         <v>886800</v>
@@ -6290,7 +6293,7 @@
         <v>281</v>
       </c>
       <c r="C279" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D279">
         <v>891160</v>
@@ -6307,7 +6310,7 @@
         <v>282</v>
       </c>
       <c r="C280" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D280">
         <v>895326</v>
@@ -6324,7 +6327,7 @@
         <v>283</v>
       </c>
       <c r="C281" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D281">
         <v>901268</v>
@@ -6341,7 +6344,7 @@
         <v>284</v>
       </c>
       <c r="C282" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D282">
         <v>906863</v>
@@ -6358,7 +6361,7 @@
         <v>285</v>
       </c>
       <c r="C283" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D283">
         <v>912811</v>
@@ -6375,7 +6378,7 @@
         <v>286</v>
       </c>
       <c r="C284" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D284">
         <v>918811</v>
@@ -6392,7 +6395,7 @@
         <v>287</v>
       </c>
       <c r="C285" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D285">
         <v>924962</v>
@@ -6409,7 +6412,7 @@
         <v>288</v>
       </c>
       <c r="C286" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D286">
         <v>929392</v>
@@ -6426,7 +6429,7 @@
         <v>289</v>
       </c>
       <c r="C287" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D287">
         <v>933155</v>
@@ -6443,7 +6446,7 @@
         <v>290</v>
       </c>
       <c r="C288" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D288">
         <v>938405</v>
@@ -6460,7 +6463,7 @@
         <v>291</v>
       </c>
       <c r="C289" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D289">
         <v>943630</v>
@@ -6477,7 +6480,7 @@
         <v>292</v>
       </c>
       <c r="C290" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D290">
         <v>949197</v>
@@ -6494,7 +6497,7 @@
         <v>293</v>
       </c>
       <c r="C291" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D291">
         <v>955128</v>
@@ -6511,7 +6514,7 @@
         <v>294</v>
       </c>
       <c r="C292" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D292">
         <v>961938</v>
@@ -6528,7 +6531,7 @@
         <v>295</v>
       </c>
       <c r="C293" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D293">
         <v>967825</v>
@@ -6545,7 +6548,7 @@
         <v>296</v>
       </c>
       <c r="C294" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D294">
         <v>972785</v>
@@ -6562,7 +6565,7 @@
         <v>297</v>
       </c>
       <c r="C295" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D295">
         <v>978531</v>
@@ -6579,7 +6582,7 @@
         <v>298</v>
       </c>
       <c r="C296" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D296">
         <v>986177</v>
@@ -6596,7 +6599,7 @@
         <v>299</v>
       </c>
       <c r="C297" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D297">
         <v>991835</v>
@@ -6613,7 +6616,7 @@
         <v>300</v>
       </c>
       <c r="C298" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D298">
         <v>997393</v>
@@ -6630,7 +6633,7 @@
         <v>301</v>
       </c>
       <c r="C299" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D299">
         <v>1003253</v>
@@ -6647,7 +6650,7 @@
         <v>302</v>
       </c>
       <c r="C300" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D300">
         <v>1006522</v>
@@ -6664,7 +6667,7 @@
         <v>303</v>
       </c>
       <c r="C301" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D301">
         <v>1009396</v>
@@ -6681,7 +6684,7 @@
         <v>304</v>
       </c>
       <c r="C302" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D302">
         <v>1011153</v>
@@ -6698,7 +6701,7 @@
         <v>305</v>
       </c>
       <c r="C303" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D303">
         <v>1015071</v>
@@ -6715,7 +6718,7 @@
         <v>306</v>
       </c>
       <c r="C304" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D304">
         <v>1019543</v>
@@ -6732,7 +6735,7 @@
         <v>307</v>
       </c>
       <c r="C305" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D305">
         <v>1025969</v>
@@ -6749,7 +6752,7 @@
         <v>308</v>
       </c>
       <c r="C306" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D306">
         <v>1032688</v>
@@ -6766,7 +6769,7 @@
         <v>309</v>
       </c>
       <c r="C307" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D307">
         <v>1041875</v>
@@ -6783,7 +6786,7 @@
         <v>310</v>
       </c>
       <c r="C308" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D308">
         <v>1049358</v>
@@ -6800,7 +6803,7 @@
         <v>311</v>
       </c>
       <c r="C309" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D309">
         <v>1060152</v>
@@ -6817,7 +6820,7 @@
         <v>312</v>
       </c>
       <c r="C310" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D310">
         <v>1070487</v>
@@ -6834,7 +6837,7 @@
         <v>313</v>
       </c>
       <c r="C311" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D311">
         <v>1078594</v>
@@ -6851,7 +6854,7 @@
         <v>314</v>
       </c>
       <c r="C312" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D312">
         <v>1090675</v>
@@ -6868,7 +6871,7 @@
         <v>315</v>
       </c>
       <c r="C313" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D313">
         <v>1101403</v>
@@ -6885,7 +6888,7 @@
         <v>316</v>
       </c>
       <c r="C314" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D314">
         <v>1107071</v>
@@ -6902,7 +6905,7 @@
         <v>317</v>
       </c>
       <c r="C315" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D315">
         <v>1113543</v>
@@ -6919,7 +6922,7 @@
         <v>318</v>
       </c>
       <c r="C316" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D316">
         <v>1122362</v>
@@ -6936,7 +6939,7 @@
         <v>319</v>
       </c>
       <c r="C317" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D317">
         <v>1133613</v>
@@ -6953,7 +6956,7 @@
         <v>320</v>
       </c>
       <c r="C318" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D318">
         <v>1144643</v>
@@ -6970,7 +6973,7 @@
         <v>321</v>
       </c>
       <c r="C319" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D319">
         <v>1156770</v>
@@ -6987,7 +6990,7 @@
         <v>322</v>
       </c>
       <c r="C320" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D320">
         <v>1168395</v>
@@ -7004,7 +7007,7 @@
         <v>323</v>
       </c>
       <c r="C321" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D321">
         <v>1175850</v>
@@ -7021,7 +7024,7 @@
         <v>324</v>
       </c>
       <c r="C322" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D322">
         <v>1182249</v>
@@ -7038,7 +7041,7 @@
         <v>325</v>
       </c>
       <c r="C323" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D323">
         <v>1193255</v>
@@ -7055,7 +7058,7 @@
         <v>326</v>
       </c>
       <c r="C324" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D324">
         <v>1205229</v>
@@ -7072,7 +7075,7 @@
         <v>327</v>
       </c>
       <c r="C325" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D325">
         <v>1217126</v>
@@ -7089,7 +7092,7 @@
         <v>328</v>
       </c>
       <c r="C326" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D326">
         <v>1229379</v>
@@ -7106,7 +7109,7 @@
         <v>329</v>
       </c>
       <c r="C327" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D327">
         <v>1241436</v>
@@ -7123,7 +7126,7 @@
         <v>330</v>
       </c>
       <c r="C328" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D328">
         <v>1250044</v>
@@ -7140,7 +7143,7 @@
         <v>331</v>
       </c>
       <c r="C329" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D329">
         <v>1255974</v>
@@ -7157,7 +7160,7 @@
         <v>332</v>
       </c>
       <c r="C330" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D330">
         <v>1267202</v>
@@ -7174,7 +7177,7 @@
         <v>333</v>
       </c>
       <c r="C331" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D331">
         <v>1277499</v>
@@ -7191,7 +7194,7 @@
         <v>334</v>
       </c>
       <c r="C332" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D332">
         <v>1289298</v>
@@ -7208,7 +7211,7 @@
         <v>335</v>
       </c>
       <c r="C333" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D333">
         <v>1301546</v>
@@ -7225,7 +7228,7 @@
         <v>336</v>
       </c>
       <c r="C334" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D334">
         <v>1313675</v>
@@ -7242,7 +7245,7 @@
         <v>337</v>
       </c>
       <c r="C335" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D335">
         <v>1320545</v>
@@ -7259,7 +7262,7 @@
         <v>338</v>
       </c>
       <c r="C336" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D336">
         <v>1325915</v>
@@ -7276,7 +7279,7 @@
         <v>339</v>
       </c>
       <c r="C337" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D337">
         <v>1338426</v>
@@ -7293,7 +7296,7 @@
         <v>340</v>
       </c>
       <c r="C338" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D338">
         <v>1350079</v>
@@ -7310,7 +7313,7 @@
         <v>341</v>
       </c>
       <c r="C339" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D339">
         <v>1362564</v>
@@ -7327,7 +7330,7 @@
         <v>342</v>
       </c>
       <c r="C340" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D340">
         <v>1372243</v>
@@ -7344,7 +7347,7 @@
         <v>343</v>
       </c>
       <c r="C341" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D341">
         <v>1377217</v>
@@ -7361,7 +7364,7 @@
         <v>344</v>
       </c>
       <c r="C342" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D342">
         <v>1383434</v>
@@ -7378,7 +7381,7 @@
         <v>345</v>
       </c>
       <c r="C343" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D343">
         <v>1389430</v>
@@ -7395,7 +7398,7 @@
         <v>346</v>
       </c>
       <c r="C344" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D344">
         <v>1401529</v>
@@ -7412,7 +7415,7 @@
         <v>347</v>
       </c>
       <c r="C345" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D345">
         <v>1413935</v>
@@ -7429,7 +7432,7 @@
         <v>348</v>
       </c>
       <c r="C346" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D346">
         <v>1426094</v>
@@ -7446,7 +7449,7 @@
         <v>349</v>
       </c>
       <c r="C347" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D347">
         <v>1437185</v>
@@ -7463,7 +7466,7 @@
         <v>350</v>
       </c>
       <c r="C348" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D348">
         <v>1443544</v>
@@ -7480,7 +7483,7 @@
         <v>351</v>
       </c>
       <c r="C349" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D349">
         <v>1448755</v>
@@ -7497,7 +7500,7 @@
         <v>352</v>
       </c>
       <c r="C350" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D350">
         <v>1455219</v>
@@ -7514,7 +7517,7 @@
         <v>353</v>
       </c>
       <c r="C351" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D351">
         <v>1466490</v>
@@ -7531,7 +7534,7 @@
         <v>354</v>
       </c>
       <c r="C352" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D352">
         <v>1479835</v>
@@ -7548,7 +7551,7 @@
         <v>355</v>
       </c>
       <c r="C353" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D353">
         <v>1493569</v>
@@ -7565,7 +7568,7 @@
         <v>356</v>
       </c>
       <c r="C354" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D354">
         <v>1507931</v>
@@ -7582,7 +7585,7 @@
         <v>357</v>
       </c>
       <c r="C355" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D355">
         <v>1524036</v>
@@ -7599,7 +7602,7 @@
         <v>358</v>
       </c>
       <c r="C356" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D356">
         <v>1534039</v>
@@ -7616,7 +7619,7 @@
         <v>359</v>
       </c>
       <c r="C357" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D357">
         <v>1541633</v>
@@ -7633,7 +7636,7 @@
         <v>360</v>
       </c>
       <c r="C358" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D358">
         <v>1556028</v>
@@ -7650,7 +7653,7 @@
         <v>361</v>
       </c>
       <c r="C359" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D359">
         <v>1571901</v>
@@ -7667,7 +7670,7 @@
         <v>362</v>
       </c>
       <c r="C360" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D360">
         <v>1588369</v>
@@ -7684,7 +7687,7 @@
         <v>363</v>
       </c>
       <c r="C361" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D361">
         <v>1609735</v>
@@ -7701,7 +7704,7 @@
         <v>364</v>
       </c>
       <c r="C362" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D362">
         <v>1630258</v>
@@ -7718,7 +7721,7 @@
         <v>365</v>
       </c>
       <c r="C363" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D363">
         <v>1641428</v>
@@ -7735,7 +7738,7 @@
         <v>366</v>
       </c>
       <c r="C364" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D364">
         <v>1649502</v>
@@ -7752,7 +7755,7 @@
         <v>367</v>
       </c>
       <c r="C365" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D365">
         <v>1668396</v>
@@ -7769,7 +7772,7 @@
         <v>368</v>
       </c>
       <c r="C366" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D366">
         <v>1688944</v>
@@ -7786,7 +7789,7 @@
         <v>369</v>
       </c>
       <c r="C367" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D367">
         <v>1711283</v>
@@ -7803,7 +7806,7 @@
         <v>370</v>
       </c>
       <c r="C368" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D368">
         <v>1732290</v>
@@ -7820,7 +7823,7 @@
         <v>371</v>
       </c>
       <c r="C369" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D369">
         <v>1752347</v>
@@ -7837,7 +7840,7 @@
         <v>372</v>
       </c>
       <c r="C370" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D370">
         <v>1763219</v>
@@ -7854,7 +7857,7 @@
         <v>373</v>
       </c>
       <c r="C371" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D371">
         <v>1771740</v>
@@ -7871,7 +7874,7 @@
         <v>374</v>
       </c>
       <c r="C372" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D372">
         <v>1788905</v>
@@ -7888,7 +7891,7 @@
         <v>375</v>
       </c>
       <c r="C373" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D373">
         <v>1806849</v>
@@ -7905,7 +7908,7 @@
         <v>376</v>
       </c>
       <c r="C374" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D374">
         <v>1825519</v>
@@ -7922,7 +7925,7 @@
         <v>377</v>
       </c>
       <c r="C375" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D375">
         <v>1841893</v>
@@ -7939,7 +7942,7 @@
         <v>378</v>
       </c>
       <c r="C376" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D376">
         <v>1857230</v>
@@ -7956,7 +7959,7 @@
         <v>379</v>
       </c>
       <c r="C377" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D377">
         <v>1864260</v>
@@ -7973,7 +7976,7 @@
         <v>380</v>
       </c>
       <c r="C378" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D378">
         <v>1869708</v>
@@ -7990,7 +7993,7 @@
         <v>381</v>
       </c>
       <c r="C379" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D379">
         <v>1874092</v>
@@ -8007,7 +8010,7 @@
         <v>382</v>
       </c>
       <c r="C380" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D380">
         <v>1886245</v>
@@ -8024,7 +8027,7 @@
         <v>383</v>
       </c>
       <c r="C381" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D381">
         <v>1886245</v>
@@ -8041,7 +8044,7 @@
         <v>384</v>
       </c>
       <c r="C382" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D382">
         <v>1912871</v>
@@ -8058,7 +8061,7 @@
         <v>385</v>
       </c>
       <c r="C383" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D383">
         <v>1926080</v>
@@ -8075,7 +8078,7 @@
         <v>386</v>
       </c>
       <c r="C384" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D384">
         <v>1932145</v>
@@ -8092,7 +8095,7 @@
         <v>387</v>
       </c>
       <c r="C385" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D385">
         <v>1936013</v>
@@ -8109,7 +8112,7 @@
         <v>388</v>
       </c>
       <c r="C386" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D386">
         <v>1946751</v>
@@ -8126,7 +8129,7 @@
         <v>389</v>
       </c>
       <c r="C387" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D387">
         <v>1957889</v>
@@ -8143,7 +8146,7 @@
         <v>390</v>
       </c>
       <c r="C388" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D388">
         <v>1968566</v>
@@ -8160,7 +8163,7 @@
         <v>391</v>
       </c>
       <c r="C389" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D389">
         <v>1978954</v>
@@ -8177,13 +8180,30 @@
         <v>392</v>
       </c>
       <c r="C390" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D390">
         <v>1988695</v>
       </c>
       <c r="E390">
         <v>173771</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5">
+      <c r="A391" s="1">
+        <v>389</v>
+      </c>
+      <c r="B391" t="s">
+        <v>393</v>
+      </c>
+      <c r="C391" t="s">
+        <v>394</v>
+      </c>
+      <c r="D391">
+        <v>1992794</v>
+      </c>
+      <c r="E391">
+        <v>174207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some graphs for COVID
</commit_message>
<xml_diff>
--- a/mexico.xlsx
+++ b/mexico.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="397">
   <si>
     <t>date</t>
   </si>
@@ -1196,6 +1196,12 @@
   </si>
   <si>
     <t>2021-02-14</t>
+  </si>
+  <si>
+    <t>2021-02-15</t>
+  </si>
+  <si>
+    <t>2021-02-16</t>
   </si>
   <si>
     <t>mexico</t>
@@ -1556,7 +1562,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E391"/>
+  <dimension ref="A1:E393"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1584,7 +1590,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1601,7 +1607,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1618,7 +1624,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1635,7 +1641,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1652,7 +1658,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1669,7 +1675,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1686,7 +1692,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1703,7 +1709,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1720,7 +1726,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1737,7 +1743,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1754,7 +1760,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1771,7 +1777,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1788,7 +1794,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1805,7 +1811,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1822,7 +1828,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1839,7 +1845,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1856,7 +1862,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1873,7 +1879,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1890,7 +1896,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1907,7 +1913,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1924,7 +1930,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1941,7 +1947,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1958,7 +1964,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1975,7 +1981,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1992,7 +1998,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2009,7 +2015,7 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2026,7 +2032,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2043,7 +2049,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2060,7 +2066,7 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2077,7 +2083,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2094,7 +2100,7 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2111,7 +2117,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2128,7 +2134,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2145,7 +2151,7 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2162,7 +2168,7 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2179,7 +2185,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2196,7 +2202,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2213,7 +2219,7 @@
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2230,7 +2236,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -2247,7 +2253,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D41">
         <v>5</v>
@@ -2264,7 +2270,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D42">
         <v>5</v>
@@ -2281,7 +2287,7 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2298,7 +2304,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D44">
         <v>5</v>
@@ -2315,7 +2321,7 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D45">
         <v>5</v>
@@ -2332,7 +2338,7 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D46">
         <v>6</v>
@@ -2349,7 +2355,7 @@
         <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D47">
         <v>6</v>
@@ -2366,7 +2372,7 @@
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D48">
         <v>7</v>
@@ -2383,7 +2389,7 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D49">
         <v>7</v>
@@ -2400,7 +2406,7 @@
         <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D50">
         <v>7</v>
@@ -2417,7 +2423,7 @@
         <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D51">
         <v>8</v>
@@ -2434,7 +2440,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D52">
         <v>12</v>
@@ -2451,7 +2457,7 @@
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D53">
         <v>26</v>
@@ -2468,7 +2474,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D54">
         <v>41</v>
@@ -2485,7 +2491,7 @@
         <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D55">
         <v>53</v>
@@ -2502,7 +2508,7 @@
         <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D56">
         <v>82</v>
@@ -2519,7 +2525,7 @@
         <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D57">
         <v>93</v>
@@ -2536,7 +2542,7 @@
         <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D58">
         <v>118</v>
@@ -2553,7 +2559,7 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D59">
         <v>164</v>
@@ -2570,7 +2576,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D60">
         <v>203</v>
@@ -2587,7 +2593,7 @@
         <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D61">
         <v>251</v>
@@ -2604,7 +2610,7 @@
         <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D62">
         <v>316</v>
@@ -2621,7 +2627,7 @@
         <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D63">
         <v>367</v>
@@ -2638,7 +2644,7 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D64">
         <v>405</v>
@@ -2655,7 +2661,7 @@
         <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D65">
         <v>475</v>
@@ -2672,7 +2678,7 @@
         <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D66">
         <v>585</v>
@@ -2689,7 +2695,7 @@
         <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D67">
         <v>717</v>
@@ -2706,7 +2712,7 @@
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D68">
         <v>848</v>
@@ -2723,7 +2729,7 @@
         <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D69">
         <v>993</v>
@@ -2740,7 +2746,7 @@
         <v>72</v>
       </c>
       <c r="C70" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D70">
         <v>1094</v>
@@ -2757,7 +2763,7 @@
         <v>73</v>
       </c>
       <c r="C71" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D71">
         <v>1215</v>
@@ -2774,7 +2780,7 @@
         <v>74</v>
       </c>
       <c r="C72" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D72">
         <v>1378</v>
@@ -2791,7 +2797,7 @@
         <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D73">
         <v>1510</v>
@@ -2808,7 +2814,7 @@
         <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D74">
         <v>1688</v>
@@ -2825,7 +2831,7 @@
         <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D75">
         <v>1890</v>
@@ -2842,7 +2848,7 @@
         <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D76">
         <v>2143</v>
@@ -2859,7 +2865,7 @@
         <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D77">
         <v>2439</v>
@@ -2876,7 +2882,7 @@
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D78">
         <v>2785</v>
@@ -2893,7 +2899,7 @@
         <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D79">
         <v>3181</v>
@@ -2910,7 +2916,7 @@
         <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D80">
         <v>3441</v>
@@ -2927,7 +2933,7 @@
         <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D81">
         <v>3844</v>
@@ -2944,7 +2950,7 @@
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D82">
         <v>4219</v>
@@ -2961,7 +2967,7 @@
         <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D83">
         <v>4661</v>
@@ -2978,7 +2984,7 @@
         <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D84">
         <v>5014</v>
@@ -2995,7 +3001,7 @@
         <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D85">
         <v>5399</v>
@@ -3012,7 +3018,7 @@
         <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D86">
         <v>5847</v>
@@ -3029,7 +3035,7 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D87">
         <v>6297</v>
@@ -3046,7 +3052,7 @@
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D88">
         <v>6875</v>
@@ -3063,7 +3069,7 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D89">
         <v>7497</v>
@@ -3080,7 +3086,7 @@
         <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D90">
         <v>8261</v>
@@ -3097,7 +3103,7 @@
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D91">
         <v>8772</v>
@@ -3114,7 +3120,7 @@
         <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D92">
         <v>9501</v>
@@ -3131,7 +3137,7 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D93">
         <v>10544</v>
@@ -3148,7 +3154,7 @@
         <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D94">
         <v>11633</v>
@@ -3165,7 +3171,7 @@
         <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D95">
         <v>12872</v>
@@ -3182,7 +3188,7 @@
         <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D96">
         <v>13842</v>
@@ -3199,7 +3205,7 @@
         <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D97">
         <v>14677</v>
@@ -3216,7 +3222,7 @@
         <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D98">
         <v>15529</v>
@@ -3233,7 +3239,7 @@
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D99">
         <v>16752</v>
@@ -3250,7 +3256,7 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D100">
         <v>17799</v>
@@ -3267,7 +3273,7 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D101">
         <v>19224</v>
@@ -3284,7 +3290,7 @@
         <v>104</v>
       </c>
       <c r="C102" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D102">
         <v>20739</v>
@@ -3301,7 +3307,7 @@
         <v>105</v>
       </c>
       <c r="C103" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D103">
         <v>22088</v>
@@ -3318,7 +3324,7 @@
         <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D104">
         <v>23471</v>
@@ -3335,7 +3341,7 @@
         <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D105">
         <v>24905</v>
@@ -3352,7 +3358,7 @@
         <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D106">
         <v>26025</v>
@@ -3369,7 +3375,7 @@
         <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D107">
         <v>27634</v>
@@ -3386,7 +3392,7 @@
         <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D108">
         <v>29616</v>
@@ -3403,7 +3409,7 @@
         <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D109">
         <v>31522</v>
@@ -3420,7 +3426,7 @@
         <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D110">
         <v>33460</v>
@@ -3437,7 +3443,7 @@
         <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D111">
         <v>35022</v>
@@ -3454,7 +3460,7 @@
         <v>114</v>
       </c>
       <c r="C112" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D112">
         <v>36327</v>
@@ -3471,7 +3477,7 @@
         <v>115</v>
       </c>
       <c r="C113" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D113">
         <v>38324</v>
@@ -3488,7 +3494,7 @@
         <v>116</v>
       </c>
       <c r="C114" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D114">
         <v>40186</v>
@@ -3505,7 +3511,7 @@
         <v>117</v>
       </c>
       <c r="C115" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D115">
         <v>42595</v>
@@ -3522,7 +3528,7 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D116">
         <v>45032</v>
@@ -3539,7 +3545,7 @@
         <v>119</v>
       </c>
       <c r="C117" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D117">
         <v>47144</v>
@@ -3556,7 +3562,7 @@
         <v>120</v>
       </c>
       <c r="C118" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D118">
         <v>49219</v>
@@ -3573,7 +3579,7 @@
         <v>121</v>
       </c>
       <c r="C119" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D119">
         <v>51633</v>
@@ -3590,7 +3596,7 @@
         <v>122</v>
       </c>
       <c r="C120" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D120">
         <v>54346</v>
@@ -3607,7 +3613,7 @@
         <v>123</v>
       </c>
       <c r="C121" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D121">
         <v>56594</v>
@@ -3624,7 +3630,7 @@
         <v>124</v>
       </c>
       <c r="C122" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D122">
         <v>59567</v>
@@ -3641,7 +3647,7 @@
         <v>125</v>
       </c>
       <c r="C123" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D123">
         <v>62527</v>
@@ -3658,7 +3664,7 @@
         <v>126</v>
       </c>
       <c r="C124" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D124">
         <v>65856</v>
@@ -3675,7 +3681,7 @@
         <v>127</v>
       </c>
       <c r="C125" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D125">
         <v>68620</v>
@@ -3692,7 +3698,7 @@
         <v>128</v>
       </c>
       <c r="C126" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D126">
         <v>71105</v>
@@ -3709,7 +3715,7 @@
         <v>129</v>
       </c>
       <c r="C127" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D127">
         <v>74560</v>
@@ -3726,7 +3732,7 @@
         <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D128">
         <v>78023</v>
@@ -3743,7 +3749,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D129">
         <v>81400</v>
@@ -3760,7 +3766,7 @@
         <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D130">
         <v>84627</v>
@@ -3777,7 +3783,7 @@
         <v>133</v>
       </c>
       <c r="C131" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D131">
         <v>87512</v>
@@ -3794,7 +3800,7 @@
         <v>134</v>
       </c>
       <c r="C132" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D132">
         <v>90664</v>
@@ -3811,7 +3817,7 @@
         <v>135</v>
       </c>
       <c r="C133" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D133">
         <v>93435</v>
@@ -3828,7 +3834,7 @@
         <v>136</v>
       </c>
       <c r="C134" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D134">
         <v>97326</v>
@@ -3845,7 +3851,7 @@
         <v>137</v>
       </c>
       <c r="C135" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D135">
         <v>101238</v>
@@ -3862,7 +3868,7 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D136">
         <v>105680</v>
@@ -3879,7 +3885,7 @@
         <v>139</v>
       </c>
       <c r="C137" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D137">
         <v>110026</v>
@@ -3896,7 +3902,7 @@
         <v>140</v>
       </c>
       <c r="C138" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D138">
         <v>113619</v>
@@ -3913,7 +3919,7 @@
         <v>141</v>
       </c>
       <c r="C139" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D139">
         <v>117103</v>
@@ -3930,7 +3936,7 @@
         <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D140">
         <v>120102</v>
@@ -3947,7 +3953,7 @@
         <v>143</v>
       </c>
       <c r="C141" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D141">
         <v>124301</v>
@@ -3964,7 +3970,7 @@
         <v>144</v>
       </c>
       <c r="C142" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D142">
         <v>129184</v>
@@ -3981,7 +3987,7 @@
         <v>145</v>
       </c>
       <c r="C143" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D143">
         <v>133974</v>
@@ -3998,7 +4004,7 @@
         <v>146</v>
       </c>
       <c r="C144" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D144">
         <v>139196</v>
@@ -4015,7 +4021,7 @@
         <v>147</v>
       </c>
       <c r="C145" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D145">
         <v>142690</v>
@@ -4032,7 +4038,7 @@
         <v>148</v>
       </c>
       <c r="C146" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D146">
         <v>146837</v>
@@ -4049,7 +4055,7 @@
         <v>149</v>
       </c>
       <c r="C147" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D147">
         <v>150264</v>
@@ -4066,7 +4072,7 @@
         <v>150</v>
       </c>
       <c r="C148" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D148">
         <v>154863</v>
@@ -4083,7 +4089,7 @@
         <v>151</v>
       </c>
       <c r="C149" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D149">
         <v>159793</v>
@@ -4100,7 +4106,7 @@
         <v>152</v>
       </c>
       <c r="C150" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D150">
         <v>165455</v>
@@ -4117,7 +4123,7 @@
         <v>153</v>
       </c>
       <c r="C151" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D151">
         <v>170485</v>
@@ -4134,7 +4140,7 @@
         <v>154</v>
       </c>
       <c r="C152" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D152">
         <v>175202</v>
@@ -4151,7 +4157,7 @@
         <v>155</v>
       </c>
       <c r="C153" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D153">
         <v>180545</v>
@@ -4168,7 +4174,7 @@
         <v>156</v>
       </c>
       <c r="C154" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D154">
         <v>185122</v>
@@ -4185,7 +4191,7 @@
         <v>157</v>
       </c>
       <c r="C155" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D155">
         <v>191410</v>
@@ -4202,7 +4208,7 @@
         <v>158</v>
       </c>
       <c r="C156" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D156">
         <v>196847</v>
@@ -4219,7 +4225,7 @@
         <v>159</v>
       </c>
       <c r="C157" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D157">
         <v>202951</v>
@@ -4236,7 +4242,7 @@
         <v>160</v>
       </c>
       <c r="C158" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D158">
         <v>208392</v>
@@ -4253,7 +4259,7 @@
         <v>161</v>
       </c>
       <c r="C159" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D159">
         <v>212802</v>
@@ -4270,7 +4276,7 @@
         <v>162</v>
       </c>
       <c r="C160" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D160">
         <v>216852</v>
@@ -4287,7 +4293,7 @@
         <v>163</v>
       </c>
       <c r="C161" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D161">
         <v>220657</v>
@@ -4304,7 +4310,7 @@
         <v>164</v>
       </c>
       <c r="C162" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D162">
         <v>226089</v>
@@ -4321,7 +4327,7 @@
         <v>165</v>
       </c>
       <c r="C163" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D163">
         <v>231770</v>
@@ -4338,7 +4344,7 @@
         <v>166</v>
       </c>
       <c r="C164" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D164">
         <v>238511</v>
@@ -4355,7 +4361,7 @@
         <v>167</v>
       </c>
       <c r="C165" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D165">
         <v>245251</v>
@@ -4372,7 +4378,7 @@
         <v>168</v>
       </c>
       <c r="C166" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D166">
         <v>252165</v>
@@ -4389,7 +4395,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D167">
         <v>256848</v>
@@ -4406,7 +4412,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D168">
         <v>261750</v>
@@ -4423,7 +4429,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D169">
         <v>268008</v>
@@ -4440,7 +4446,7 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D170">
         <v>275003</v>
@@ -4457,7 +4463,7 @@
         <v>173</v>
       </c>
       <c r="C171" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D171">
         <v>282283</v>
@@ -4474,7 +4480,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D172">
         <v>289174</v>
@@ -4491,7 +4497,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D173">
         <v>295268</v>
@@ -4508,7 +4514,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D174">
         <v>299750</v>
@@ -4525,7 +4531,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D175">
         <v>304435</v>
@@ -4542,7 +4548,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D176">
         <v>311486</v>
@@ -4559,7 +4565,7 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D177">
         <v>317635</v>
@@ -4576,7 +4582,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D178">
         <v>324041</v>
@@ -4593,7 +4599,7 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D179">
         <v>331298</v>
@@ -4610,7 +4616,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D180">
         <v>338913</v>
@@ -4627,7 +4633,7 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D181">
         <v>344224</v>
@@ -4644,7 +4650,7 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D182">
         <v>349396</v>
@@ -4661,7 +4667,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D183">
         <v>356255</v>
@@ -4678,7 +4684,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D184">
         <v>362274</v>
@@ -4695,7 +4701,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D185">
         <v>370712</v>
@@ -4712,7 +4718,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D186">
         <v>378285</v>
@@ -4729,7 +4735,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D187">
         <v>385036</v>
@@ -4746,7 +4752,7 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D188">
         <v>390516</v>
@@ -4763,7 +4769,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D189">
         <v>395489</v>
@@ -4780,7 +4786,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D190">
         <v>402697</v>
@@ -4797,7 +4803,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D191">
         <v>408449</v>
@@ -4814,7 +4820,7 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D192">
         <v>416179</v>
@@ -4831,7 +4837,7 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D193">
         <v>424637</v>
@@ -4848,7 +4854,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D194">
         <v>434193</v>
@@ -4865,7 +4871,7 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D195">
         <v>439046</v>
@@ -4882,7 +4888,7 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D196">
         <v>443813</v>
@@ -4899,7 +4905,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D197">
         <v>449961</v>
@@ -4916,7 +4922,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D198">
         <v>456100</v>
@@ -4933,7 +4939,7 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D199">
         <v>462690</v>
@@ -4950,7 +4956,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D200">
         <v>469407</v>
@@ -4967,7 +4973,7 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D201">
         <v>475902</v>
@@ -4984,7 +4990,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D202">
         <v>480278</v>
@@ -5001,7 +5007,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D203">
         <v>485836</v>
@@ -5018,7 +5024,7 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D204">
         <v>492522</v>
@@ -5035,7 +5041,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D205">
         <v>498380</v>
@@ -5052,7 +5058,7 @@
         <v>208</v>
       </c>
       <c r="C206" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D206">
         <v>505751</v>
@@ -5069,7 +5075,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D207">
         <v>511369</v>
@@ -5086,7 +5092,7 @@
         <v>210</v>
       </c>
       <c r="C208" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D208">
         <v>517714</v>
@@ -5103,7 +5109,7 @@
         <v>211</v>
       </c>
       <c r="C209" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D209">
         <v>522162</v>
@@ -5120,7 +5126,7 @@
         <v>212</v>
       </c>
       <c r="C210" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D210">
         <v>525733</v>
@@ -5137,7 +5143,7 @@
         <v>213</v>
       </c>
       <c r="C211" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D211">
         <v>531239</v>
@@ -5154,7 +5160,7 @@
         <v>214</v>
       </c>
       <c r="C212" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D212">
         <v>537031</v>
@@ -5171,7 +5177,7 @@
         <v>215</v>
       </c>
       <c r="C213" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D213">
         <v>543806</v>
@@ -5188,7 +5194,7 @@
         <v>216</v>
       </c>
       <c r="C214" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D214">
         <v>549734</v>
@@ -5205,7 +5211,7 @@
         <v>217</v>
       </c>
       <c r="C215" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D215">
         <v>556216</v>
@@ -5222,7 +5228,7 @@
         <v>218</v>
       </c>
       <c r="C216" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D216">
         <v>560164</v>
@@ -5239,7 +5245,7 @@
         <v>219</v>
       </c>
       <c r="C217" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D217">
         <v>563705</v>
@@ -5256,7 +5262,7 @@
         <v>220</v>
       </c>
       <c r="C218" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D218">
         <v>568621</v>
@@ -5273,7 +5279,7 @@
         <v>221</v>
       </c>
       <c r="C219" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D219">
         <v>573888</v>
@@ -5290,7 +5296,7 @@
         <v>222</v>
       </c>
       <c r="C220" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D220">
         <v>579914</v>
@@ -5307,7 +5313,7 @@
         <v>223</v>
       </c>
       <c r="C221" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D221">
         <v>585738</v>
@@ -5324,7 +5330,7 @@
         <v>224</v>
       </c>
       <c r="C222" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D222">
         <v>591712</v>
@@ -5341,7 +5347,7 @@
         <v>225</v>
       </c>
       <c r="C223" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D223">
         <v>595841</v>
@@ -5358,7 +5364,7 @@
         <v>226</v>
       </c>
       <c r="C224" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D224">
         <v>599560</v>
@@ -5375,7 +5381,7 @@
         <v>227</v>
       </c>
       <c r="C225" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D225">
         <v>606036</v>
@@ -5392,7 +5398,7 @@
         <v>228</v>
       </c>
       <c r="C226" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D226">
         <v>610957</v>
@@ -5409,7 +5415,7 @@
         <v>229</v>
       </c>
       <c r="C227" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D227">
         <v>616894</v>
@@ -5426,7 +5432,7 @@
         <v>230</v>
       </c>
       <c r="C228" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D228">
         <v>623090</v>
@@ -5443,7 +5449,7 @@
         <v>231</v>
       </c>
       <c r="C229" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D229">
         <v>629409</v>
@@ -5460,7 +5466,7 @@
         <v>232</v>
       </c>
       <c r="C230" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D230">
         <v>634023</v>
@@ -5477,7 +5483,7 @@
         <v>233</v>
       </c>
       <c r="C231" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D231">
         <v>637509</v>
@@ -5494,7 +5500,7 @@
         <v>234</v>
       </c>
       <c r="C232" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D232">
         <v>642860</v>
@@ -5511,7 +5517,7 @@
         <v>235</v>
       </c>
       <c r="C233" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D233">
         <v>647321</v>
@@ -5528,7 +5534,7 @@
         <v>236</v>
       </c>
       <c r="C234" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D234">
         <v>652364</v>
@@ -5545,7 +5551,7 @@
         <v>237</v>
       </c>
       <c r="C235" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D235">
         <v>658299</v>
@@ -5562,7 +5568,7 @@
         <v>238</v>
       </c>
       <c r="C236" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D236">
         <v>663973</v>
@@ -5579,7 +5585,7 @@
         <v>239</v>
       </c>
       <c r="C237" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D237">
         <v>668381</v>
@@ -5596,7 +5602,7 @@
         <v>240</v>
       </c>
       <c r="C238" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D238">
         <v>671716</v>
@@ -5613,7 +5619,7 @@
         <v>241</v>
       </c>
       <c r="C239" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D239">
         <v>676487</v>
@@ -5630,7 +5636,7 @@
         <v>242</v>
       </c>
       <c r="C240" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D240">
         <v>680931</v>
@@ -5647,7 +5653,7 @@
         <v>243</v>
       </c>
       <c r="C241" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D241">
         <v>684113</v>
@@ -5664,7 +5670,7 @@
         <v>244</v>
       </c>
       <c r="C242" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D242">
         <v>688954</v>
@@ -5681,7 +5687,7 @@
         <v>245</v>
       </c>
       <c r="C243" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D243">
         <v>694121</v>
@@ -5698,7 +5704,7 @@
         <v>246</v>
       </c>
       <c r="C244" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D244">
         <v>697663</v>
@@ -5715,7 +5721,7 @@
         <v>247</v>
       </c>
       <c r="C245" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D245">
         <v>700580</v>
@@ -5732,7 +5738,7 @@
         <v>248</v>
       </c>
       <c r="C246" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D246">
         <v>705263</v>
@@ -5749,7 +5755,7 @@
         <v>249</v>
       </c>
       <c r="C247" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D247">
         <v>710049</v>
@@ -5766,7 +5772,7 @@
         <v>250</v>
       </c>
       <c r="C248" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D248">
         <v>715457</v>
@@ -5783,7 +5789,7 @@
         <v>251</v>
       </c>
       <c r="C249" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D249">
         <v>720858</v>
@@ -5800,7 +5806,7 @@
         <v>252</v>
       </c>
       <c r="C250" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D250">
         <v>726431</v>
@@ -5817,7 +5823,7 @@
         <v>253</v>
       </c>
       <c r="C251" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D251">
         <v>730317</v>
@@ -5834,7 +5840,7 @@
         <v>254</v>
       </c>
       <c r="C252" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D252">
         <v>733717</v>
@@ -5851,7 +5857,7 @@
         <v>255</v>
       </c>
       <c r="C253" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D253">
         <v>738163</v>
@@ -5868,7 +5874,7 @@
         <v>256</v>
       </c>
       <c r="C254" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D254">
         <v>743216</v>
@@ -5885,7 +5891,7 @@
         <v>257</v>
       </c>
       <c r="C255" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D255">
         <v>748315</v>
@@ -5902,7 +5908,7 @@
         <v>258</v>
       </c>
       <c r="C256" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D256">
         <v>753090</v>
@@ -5919,7 +5925,7 @@
         <v>259</v>
       </c>
       <c r="C257" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D257">
         <v>757953</v>
@@ -5936,7 +5942,7 @@
         <v>260</v>
       </c>
       <c r="C258" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D258">
         <v>761665</v>
@@ -5953,7 +5959,7 @@
         <v>261</v>
       </c>
       <c r="C259" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D259">
         <v>789780</v>
@@ -5970,7 +5976,7 @@
         <v>262</v>
       </c>
       <c r="C260" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D260">
         <v>794608</v>
@@ -5987,7 +5993,7 @@
         <v>263</v>
       </c>
       <c r="C261" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D261">
         <v>799188</v>
@@ -6004,7 +6010,7 @@
         <v>264</v>
       </c>
       <c r="C262" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D262">
         <v>804488</v>
@@ -6021,7 +6027,7 @@
         <v>265</v>
       </c>
       <c r="C263" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D263">
         <v>810020</v>
@@ -6038,7 +6044,7 @@
         <v>266</v>
       </c>
       <c r="C264" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D264">
         <v>814328</v>
@@ -6055,7 +6061,7 @@
         <v>267</v>
       </c>
       <c r="C265" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D265">
         <v>817503</v>
@@ -6072,7 +6078,7 @@
         <v>268</v>
       </c>
       <c r="C266" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D266">
         <v>821045</v>
@@ -6089,7 +6095,7 @@
         <v>269</v>
       </c>
       <c r="C267" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D267">
         <v>825340</v>
@@ -6106,7 +6112,7 @@
         <v>270</v>
       </c>
       <c r="C268" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D268">
         <v>829396</v>
@@ -6123,7 +6129,7 @@
         <v>271</v>
       </c>
       <c r="C269" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D269">
         <v>834910</v>
@@ -6140,7 +6146,7 @@
         <v>272</v>
       </c>
       <c r="C270" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D270">
         <v>841661</v>
@@ -6157,7 +6163,7 @@
         <v>273</v>
       </c>
       <c r="C271" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D271">
         <v>847108</v>
@@ -6174,7 +6180,7 @@
         <v>274</v>
       </c>
       <c r="C272" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D272">
         <v>851227</v>
@@ -6191,7 +6197,7 @@
         <v>275</v>
       </c>
       <c r="C273" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D273">
         <v>854926</v>
@@ -6208,7 +6214,7 @@
         <v>276</v>
       </c>
       <c r="C274" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D274">
         <v>860714</v>
@@ -6225,7 +6231,7 @@
         <v>277</v>
       </c>
       <c r="C275" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D275">
         <v>867559</v>
@@ -6242,7 +6248,7 @@
         <v>278</v>
       </c>
       <c r="C276" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D276">
         <v>874171</v>
@@ -6259,7 +6265,7 @@
         <v>279</v>
       </c>
       <c r="C277" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D277">
         <v>880775</v>
@@ -6276,7 +6282,7 @@
         <v>280</v>
       </c>
       <c r="C278" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D278">
         <v>886800</v>
@@ -6293,7 +6299,7 @@
         <v>281</v>
       </c>
       <c r="C279" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D279">
         <v>891160</v>
@@ -6310,7 +6316,7 @@
         <v>282</v>
       </c>
       <c r="C280" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D280">
         <v>895326</v>
@@ -6327,7 +6333,7 @@
         <v>283</v>
       </c>
       <c r="C281" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D281">
         <v>901268</v>
@@ -6344,7 +6350,7 @@
         <v>284</v>
       </c>
       <c r="C282" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D282">
         <v>906863</v>
@@ -6361,7 +6367,7 @@
         <v>285</v>
       </c>
       <c r="C283" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D283">
         <v>912811</v>
@@ -6378,7 +6384,7 @@
         <v>286</v>
       </c>
       <c r="C284" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D284">
         <v>918811</v>
@@ -6395,7 +6401,7 @@
         <v>287</v>
       </c>
       <c r="C285" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D285">
         <v>924962</v>
@@ -6412,7 +6418,7 @@
         <v>288</v>
       </c>
       <c r="C286" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D286">
         <v>929392</v>
@@ -6429,7 +6435,7 @@
         <v>289</v>
       </c>
       <c r="C287" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D287">
         <v>933155</v>
@@ -6446,7 +6452,7 @@
         <v>290</v>
       </c>
       <c r="C288" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D288">
         <v>938405</v>
@@ -6463,7 +6469,7 @@
         <v>291</v>
       </c>
       <c r="C289" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D289">
         <v>943630</v>
@@ -6480,7 +6486,7 @@
         <v>292</v>
       </c>
       <c r="C290" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D290">
         <v>949197</v>
@@ -6497,7 +6503,7 @@
         <v>293</v>
       </c>
       <c r="C291" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D291">
         <v>955128</v>
@@ -6514,7 +6520,7 @@
         <v>294</v>
       </c>
       <c r="C292" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D292">
         <v>961938</v>
@@ -6531,7 +6537,7 @@
         <v>295</v>
       </c>
       <c r="C293" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D293">
         <v>967825</v>
@@ -6548,7 +6554,7 @@
         <v>296</v>
       </c>
       <c r="C294" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D294">
         <v>972785</v>
@@ -6565,7 +6571,7 @@
         <v>297</v>
       </c>
       <c r="C295" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D295">
         <v>978531</v>
@@ -6582,7 +6588,7 @@
         <v>298</v>
       </c>
       <c r="C296" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D296">
         <v>986177</v>
@@ -6599,7 +6605,7 @@
         <v>299</v>
       </c>
       <c r="C297" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D297">
         <v>991835</v>
@@ -6616,7 +6622,7 @@
         <v>300</v>
       </c>
       <c r="C298" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D298">
         <v>997393</v>
@@ -6633,7 +6639,7 @@
         <v>301</v>
       </c>
       <c r="C299" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D299">
         <v>1003253</v>
@@ -6650,7 +6656,7 @@
         <v>302</v>
       </c>
       <c r="C300" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D300">
         <v>1006522</v>
@@ -6667,7 +6673,7 @@
         <v>303</v>
       </c>
       <c r="C301" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D301">
         <v>1009396</v>
@@ -6684,7 +6690,7 @@
         <v>304</v>
       </c>
       <c r="C302" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D302">
         <v>1011153</v>
@@ -6701,7 +6707,7 @@
         <v>305</v>
       </c>
       <c r="C303" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D303">
         <v>1015071</v>
@@ -6718,7 +6724,7 @@
         <v>306</v>
       </c>
       <c r="C304" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D304">
         <v>1019543</v>
@@ -6735,7 +6741,7 @@
         <v>307</v>
       </c>
       <c r="C305" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D305">
         <v>1025969</v>
@@ -6752,7 +6758,7 @@
         <v>308</v>
       </c>
       <c r="C306" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D306">
         <v>1032688</v>
@@ -6769,7 +6775,7 @@
         <v>309</v>
       </c>
       <c r="C307" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D307">
         <v>1041875</v>
@@ -6786,7 +6792,7 @@
         <v>310</v>
       </c>
       <c r="C308" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D308">
         <v>1049358</v>
@@ -6803,7 +6809,7 @@
         <v>311</v>
       </c>
       <c r="C309" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D309">
         <v>1060152</v>
@@ -6820,7 +6826,7 @@
         <v>312</v>
       </c>
       <c r="C310" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D310">
         <v>1070487</v>
@@ -6837,7 +6843,7 @@
         <v>313</v>
       </c>
       <c r="C311" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D311">
         <v>1078594</v>
@@ -6854,7 +6860,7 @@
         <v>314</v>
       </c>
       <c r="C312" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D312">
         <v>1090675</v>
@@ -6871,7 +6877,7 @@
         <v>315</v>
       </c>
       <c r="C313" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D313">
         <v>1101403</v>
@@ -6888,7 +6894,7 @@
         <v>316</v>
       </c>
       <c r="C314" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D314">
         <v>1107071</v>
@@ -6905,7 +6911,7 @@
         <v>317</v>
       </c>
       <c r="C315" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D315">
         <v>1113543</v>
@@ -6922,7 +6928,7 @@
         <v>318</v>
       </c>
       <c r="C316" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D316">
         <v>1122362</v>
@@ -6939,7 +6945,7 @@
         <v>319</v>
       </c>
       <c r="C317" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D317">
         <v>1133613</v>
@@ -6956,7 +6962,7 @@
         <v>320</v>
       </c>
       <c r="C318" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D318">
         <v>1144643</v>
@@ -6973,7 +6979,7 @@
         <v>321</v>
       </c>
       <c r="C319" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D319">
         <v>1156770</v>
@@ -6990,7 +6996,7 @@
         <v>322</v>
       </c>
       <c r="C320" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D320">
         <v>1168395</v>
@@ -7007,7 +7013,7 @@
         <v>323</v>
       </c>
       <c r="C321" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D321">
         <v>1175850</v>
@@ -7024,7 +7030,7 @@
         <v>324</v>
       </c>
       <c r="C322" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D322">
         <v>1182249</v>
@@ -7041,7 +7047,7 @@
         <v>325</v>
       </c>
       <c r="C323" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D323">
         <v>1193255</v>
@@ -7058,7 +7064,7 @@
         <v>326</v>
       </c>
       <c r="C324" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D324">
         <v>1205229</v>
@@ -7075,7 +7081,7 @@
         <v>327</v>
       </c>
       <c r="C325" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D325">
         <v>1217126</v>
@@ -7092,7 +7098,7 @@
         <v>328</v>
       </c>
       <c r="C326" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D326">
         <v>1229379</v>
@@ -7109,7 +7115,7 @@
         <v>329</v>
       </c>
       <c r="C327" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D327">
         <v>1241436</v>
@@ -7126,7 +7132,7 @@
         <v>330</v>
       </c>
       <c r="C328" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D328">
         <v>1250044</v>
@@ -7143,7 +7149,7 @@
         <v>331</v>
       </c>
       <c r="C329" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D329">
         <v>1255974</v>
@@ -7160,7 +7166,7 @@
         <v>332</v>
       </c>
       <c r="C330" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D330">
         <v>1267202</v>
@@ -7177,7 +7183,7 @@
         <v>333</v>
       </c>
       <c r="C331" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D331">
         <v>1277499</v>
@@ -7194,7 +7200,7 @@
         <v>334</v>
       </c>
       <c r="C332" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D332">
         <v>1289298</v>
@@ -7211,7 +7217,7 @@
         <v>335</v>
       </c>
       <c r="C333" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D333">
         <v>1301546</v>
@@ -7228,7 +7234,7 @@
         <v>336</v>
       </c>
       <c r="C334" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D334">
         <v>1313675</v>
@@ -7245,7 +7251,7 @@
         <v>337</v>
       </c>
       <c r="C335" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D335">
         <v>1320545</v>
@@ -7262,7 +7268,7 @@
         <v>338</v>
       </c>
       <c r="C336" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D336">
         <v>1325915</v>
@@ -7279,7 +7285,7 @@
         <v>339</v>
       </c>
       <c r="C337" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D337">
         <v>1338426</v>
@@ -7296,7 +7302,7 @@
         <v>340</v>
       </c>
       <c r="C338" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D338">
         <v>1350079</v>
@@ -7313,7 +7319,7 @@
         <v>341</v>
       </c>
       <c r="C339" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D339">
         <v>1362564</v>
@@ -7330,7 +7336,7 @@
         <v>342</v>
       </c>
       <c r="C340" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D340">
         <v>1372243</v>
@@ -7347,7 +7353,7 @@
         <v>343</v>
       </c>
       <c r="C341" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D341">
         <v>1377217</v>
@@ -7364,7 +7370,7 @@
         <v>344</v>
       </c>
       <c r="C342" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D342">
         <v>1383434</v>
@@ -7381,7 +7387,7 @@
         <v>345</v>
       </c>
       <c r="C343" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D343">
         <v>1389430</v>
@@ -7398,7 +7404,7 @@
         <v>346</v>
       </c>
       <c r="C344" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D344">
         <v>1401529</v>
@@ -7415,7 +7421,7 @@
         <v>347</v>
       </c>
       <c r="C345" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D345">
         <v>1413935</v>
@@ -7432,7 +7438,7 @@
         <v>348</v>
       </c>
       <c r="C346" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D346">
         <v>1426094</v>
@@ -7449,7 +7455,7 @@
         <v>349</v>
       </c>
       <c r="C347" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D347">
         <v>1437185</v>
@@ -7466,7 +7472,7 @@
         <v>350</v>
       </c>
       <c r="C348" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D348">
         <v>1443544</v>
@@ -7483,7 +7489,7 @@
         <v>351</v>
       </c>
       <c r="C349" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D349">
         <v>1448755</v>
@@ -7500,7 +7506,7 @@
         <v>352</v>
       </c>
       <c r="C350" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D350">
         <v>1455219</v>
@@ -7517,7 +7523,7 @@
         <v>353</v>
       </c>
       <c r="C351" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D351">
         <v>1466490</v>
@@ -7534,7 +7540,7 @@
         <v>354</v>
       </c>
       <c r="C352" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D352">
         <v>1479835</v>
@@ -7551,7 +7557,7 @@
         <v>355</v>
       </c>
       <c r="C353" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D353">
         <v>1493569</v>
@@ -7568,7 +7574,7 @@
         <v>356</v>
       </c>
       <c r="C354" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D354">
         <v>1507931</v>
@@ -7585,7 +7591,7 @@
         <v>357</v>
       </c>
       <c r="C355" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D355">
         <v>1524036</v>
@@ -7602,7 +7608,7 @@
         <v>358</v>
       </c>
       <c r="C356" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D356">
         <v>1534039</v>
@@ -7619,7 +7625,7 @@
         <v>359</v>
       </c>
       <c r="C357" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D357">
         <v>1541633</v>
@@ -7636,7 +7642,7 @@
         <v>360</v>
       </c>
       <c r="C358" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D358">
         <v>1556028</v>
@@ -7653,7 +7659,7 @@
         <v>361</v>
       </c>
       <c r="C359" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D359">
         <v>1571901</v>
@@ -7670,7 +7676,7 @@
         <v>362</v>
       </c>
       <c r="C360" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D360">
         <v>1588369</v>
@@ -7687,7 +7693,7 @@
         <v>363</v>
       </c>
       <c r="C361" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D361">
         <v>1609735</v>
@@ -7704,7 +7710,7 @@
         <v>364</v>
       </c>
       <c r="C362" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D362">
         <v>1630258</v>
@@ -7721,7 +7727,7 @@
         <v>365</v>
       </c>
       <c r="C363" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D363">
         <v>1641428</v>
@@ -7738,7 +7744,7 @@
         <v>366</v>
       </c>
       <c r="C364" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D364">
         <v>1649502</v>
@@ -7755,7 +7761,7 @@
         <v>367</v>
       </c>
       <c r="C365" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D365">
         <v>1668396</v>
@@ -7772,7 +7778,7 @@
         <v>368</v>
       </c>
       <c r="C366" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D366">
         <v>1688944</v>
@@ -7789,7 +7795,7 @@
         <v>369</v>
       </c>
       <c r="C367" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D367">
         <v>1711283</v>
@@ -7806,7 +7812,7 @@
         <v>370</v>
       </c>
       <c r="C368" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D368">
         <v>1732290</v>
@@ -7823,7 +7829,7 @@
         <v>371</v>
       </c>
       <c r="C369" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D369">
         <v>1752347</v>
@@ -7840,7 +7846,7 @@
         <v>372</v>
       </c>
       <c r="C370" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D370">
         <v>1763219</v>
@@ -7857,7 +7863,7 @@
         <v>373</v>
       </c>
       <c r="C371" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D371">
         <v>1771740</v>
@@ -7874,7 +7880,7 @@
         <v>374</v>
       </c>
       <c r="C372" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D372">
         <v>1788905</v>
@@ -7891,7 +7897,7 @@
         <v>375</v>
       </c>
       <c r="C373" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D373">
         <v>1806849</v>
@@ -7908,7 +7914,7 @@
         <v>376</v>
       </c>
       <c r="C374" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D374">
         <v>1825519</v>
@@ -7925,7 +7931,7 @@
         <v>377</v>
       </c>
       <c r="C375" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D375">
         <v>1841893</v>
@@ -7942,7 +7948,7 @@
         <v>378</v>
       </c>
       <c r="C376" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D376">
         <v>1857230</v>
@@ -7959,7 +7965,7 @@
         <v>379</v>
       </c>
       <c r="C377" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D377">
         <v>1864260</v>
@@ -7976,7 +7982,7 @@
         <v>380</v>
       </c>
       <c r="C378" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D378">
         <v>1869708</v>
@@ -7993,7 +7999,7 @@
         <v>381</v>
       </c>
       <c r="C379" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D379">
         <v>1874092</v>
@@ -8010,7 +8016,7 @@
         <v>382</v>
       </c>
       <c r="C380" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D380">
         <v>1886245</v>
@@ -8027,7 +8033,7 @@
         <v>383</v>
       </c>
       <c r="C381" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D381">
         <v>1886245</v>
@@ -8044,7 +8050,7 @@
         <v>384</v>
       </c>
       <c r="C382" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D382">
         <v>1912871</v>
@@ -8061,7 +8067,7 @@
         <v>385</v>
       </c>
       <c r="C383" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D383">
         <v>1926080</v>
@@ -8078,7 +8084,7 @@
         <v>386</v>
       </c>
       <c r="C384" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D384">
         <v>1932145</v>
@@ -8095,7 +8101,7 @@
         <v>387</v>
       </c>
       <c r="C385" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D385">
         <v>1936013</v>
@@ -8112,7 +8118,7 @@
         <v>388</v>
       </c>
       <c r="C386" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D386">
         <v>1946751</v>
@@ -8129,7 +8135,7 @@
         <v>389</v>
       </c>
       <c r="C387" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D387">
         <v>1957889</v>
@@ -8146,7 +8152,7 @@
         <v>390</v>
       </c>
       <c r="C388" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D388">
         <v>1968566</v>
@@ -8163,7 +8169,7 @@
         <v>391</v>
       </c>
       <c r="C389" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D389">
         <v>1978954</v>
@@ -8180,7 +8186,7 @@
         <v>392</v>
       </c>
       <c r="C390" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D390">
         <v>1988695</v>
@@ -8197,13 +8203,47 @@
         <v>393</v>
       </c>
       <c r="C391" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D391">
         <v>1992794</v>
       </c>
       <c r="E391">
         <v>174207</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5">
+      <c r="A392" s="1">
+        <v>390</v>
+      </c>
+      <c r="B392" t="s">
+        <v>394</v>
+      </c>
+      <c r="C392" t="s">
+        <v>396</v>
+      </c>
+      <c r="D392">
+        <v>1995892</v>
+      </c>
+      <c r="E392">
+        <v>174657</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5">
+      <c r="A393" s="1">
+        <v>391</v>
+      </c>
+      <c r="B393" t="s">
+        <v>395</v>
+      </c>
+      <c r="C393" t="s">
+        <v>396</v>
+      </c>
+      <c r="D393">
+        <v>2004575</v>
+      </c>
+      <c r="E393">
+        <v>175986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>